<commit_message>
feat: tratamento dos dados NOVEMBRO 2022
Tratamento concluído.
</commit_message>
<xml_diff>
--- a/Base de Dados/Dados Tratados/NOVEMBRO_2022.xlsx
+++ b/Base de Dados/Dados Tratados/NOVEMBRO_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\GitHub\Projeto-Painel-de-BI-Dados-Agricolas\Base de Dados\Dados Tratados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099569F2-7D62-490E-8983-B9AD6D47FEEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB4C557-812C-491F-A053-C8B8FB9FC58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AREA_POR_PRODUTO" sheetId="1" r:id="rId1"/>
@@ -1129,7 +1129,9 @@
     <tableColumn id="22" xr3:uid="{49B2C1E3-0396-4037-BB4B-32C18FDB6CC7}" name="CEVADA" dataDxfId="5"/>
     <tableColumn id="23" xr3:uid="{C10C34AB-D106-4FB2-B097-C90EF653E9E5}" name="TRIGO" dataDxfId="4"/>
     <tableColumn id="24" xr3:uid="{80045204-E6E2-42D6-9449-CCD3B9641988}" name="TRITICALE" dataDxfId="3"/>
-    <tableColumn id="25" xr3:uid="{0FB9C96B-75F4-4026-A109-A799A828C96B}" name="GERAL" dataDxfId="2"/>
+    <tableColumn id="25" xr3:uid="{0FB9C96B-75F4-4026-A109-A799A828C96B}" name="GERAL" dataDxfId="2">
+      <calculatedColumnFormula>SUM(B2,E2:F2,I2,M2:X2)</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="26" xr3:uid="{FA0650E0-02EE-433A-927B-8DCFAD627C43}" name="ANO"/>
     <tableColumn id="27" xr3:uid="{94C00EC6-AB2D-4D90-B787-2C1FF57B5832}" name="MÊS" dataDxfId="1"/>
     <tableColumn id="28" xr3:uid="{57AFB38B-E07E-457A-9571-EB539326E109}" name="SAFRA" dataDxfId="0"/>
@@ -10675,7 +10677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BCD6B43-6B79-4F6C-BEBB-EEE94FDB59C5}">
   <dimension ref="A1:AM36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:Y36"/>
     </sheetView>
   </sheetViews>
@@ -13830,8 +13832,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A92389E-F363-478C-8FE0-DB1A38F4DB64}">
   <dimension ref="A1:AM25"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:AJ25"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AD1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B2" sqref="B2:AJ25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13840,6 +13843,7 @@
     <col min="9" max="9" width="9" customWidth="1"/>
     <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="14.42578125" bestFit="1" customWidth="1"/>
@@ -13971,13 +13975,13 @@
         <v>35</v>
       </c>
       <c r="B2" s="1">
-        <v>0</v>
+        <v>53.400000000000006</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
       </c>
       <c r="D2" s="1">
-        <v>0</v>
+        <v>31.6</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
@@ -13992,58 +13996,58 @@
         <v>0</v>
       </c>
       <c r="I2" s="1">
-        <v>0</v>
+        <v>21.8</v>
       </c>
       <c r="J2" s="1">
-        <v>0</v>
+        <v>1665.2</v>
       </c>
       <c r="K2" s="1">
-        <v>0</v>
+        <v>123.6</v>
       </c>
       <c r="L2" s="1">
-        <v>0</v>
+        <v>70.7</v>
       </c>
       <c r="M2" s="1">
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="N2" s="1">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="O2" s="1">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="P2" s="1">
         <v>0</v>
       </c>
       <c r="Q2" s="1">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="R2" s="1">
         <v>0</v>
       </c>
       <c r="S2" s="1">
-        <v>0</v>
+        <v>1463.9</v>
       </c>
       <c r="T2" s="1">
-        <v>0</v>
+        <v>5347.3</v>
       </c>
       <c r="U2" s="1">
-        <v>0</v>
+        <v>5082.8999999999996</v>
       </c>
       <c r="V2" s="1">
-        <v>0</v>
+        <v>141.6</v>
       </c>
       <c r="W2" s="1">
-        <v>0</v>
+        <v>122.8</v>
       </c>
       <c r="X2" s="1">
         <v>0</v>
       </c>
       <c r="Y2" s="1">
-        <v>0</v>
+        <v>162.60000000000002</v>
       </c>
       <c r="Z2" s="1">
-        <v>0</v>
+        <v>116.9</v>
       </c>
       <c r="AA2" s="1">
         <v>0</v>
@@ -14052,13 +14056,13 @@
         <v>0</v>
       </c>
       <c r="AC2" s="1">
-        <v>0</v>
+        <v>45.7</v>
       </c>
       <c r="AD2" s="1">
-        <v>0</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="AE2" s="1">
-        <v>0</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="AF2" s="1">
         <v>0</v>
@@ -14067,13 +14071,13 @@
         <v>0</v>
       </c>
       <c r="AH2" s="1">
-        <v>0</v>
+        <v>1718.6000000000001</v>
       </c>
       <c r="AI2" s="1">
-        <v>0</v>
+        <v>5514.8</v>
       </c>
       <c r="AJ2" s="1">
-        <v>0</v>
+        <v>7233.4000000000005</v>
       </c>
       <c r="AK2" s="2">
         <v>2022</v>
@@ -14090,13 +14094,13 @@
         <v>36</v>
       </c>
       <c r="B3" s="1">
-        <v>0</v>
+        <v>20.7</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
       </c>
       <c r="D3" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
@@ -14111,58 +14115,58 @@
         <v>0</v>
       </c>
       <c r="I3" s="1">
-        <v>0</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="J3" s="1">
-        <v>0</v>
+        <v>682.40000000000009</v>
       </c>
       <c r="K3" s="1">
-        <v>0</v>
+        <v>50.7</v>
       </c>
       <c r="L3" s="1">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="M3" s="1">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="N3" s="1">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="O3" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P3" s="1">
         <v>0</v>
       </c>
       <c r="Q3" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R3" s="1">
         <v>0</v>
       </c>
       <c r="S3" s="1">
-        <v>0</v>
+        <v>600.20000000000005</v>
       </c>
       <c r="T3" s="1">
-        <v>0</v>
+        <v>2206.8999999999996</v>
       </c>
       <c r="U3" s="1">
-        <v>0</v>
+        <v>2099.1999999999998</v>
       </c>
       <c r="V3" s="1">
-        <v>0</v>
+        <v>58.6</v>
       </c>
       <c r="W3" s="1">
-        <v>0</v>
+        <v>49.1</v>
       </c>
       <c r="X3" s="1">
         <v>0</v>
       </c>
       <c r="Y3" s="1">
-        <v>0</v>
+        <v>67.900000000000006</v>
       </c>
       <c r="Z3" s="1">
-        <v>0</v>
+        <v>47.7</v>
       </c>
       <c r="AA3" s="1">
         <v>0</v>
@@ -14171,13 +14175,13 @@
         <v>0</v>
       </c>
       <c r="AC3" s="1">
-        <v>0</v>
+        <v>20.2</v>
       </c>
       <c r="AD3" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE3" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF3" s="1">
         <v>0</v>
@@ -14186,13 +14190,13 @@
         <v>0</v>
       </c>
       <c r="AH3" s="1">
-        <v>0</v>
+        <v>703.10000000000014</v>
       </c>
       <c r="AI3" s="1">
-        <v>0</v>
+        <v>2276.7999999999997</v>
       </c>
       <c r="AJ3" s="1">
-        <v>0</v>
+        <v>2979.9</v>
       </c>
       <c r="AK3" s="2">
         <v>2022</v>
@@ -14209,13 +14213,13 @@
         <v>37</v>
       </c>
       <c r="B4" s="1">
-        <v>0</v>
+        <v>32.700000000000003</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
@@ -14230,58 +14234,58 @@
         <v>0</v>
       </c>
       <c r="I4" s="1">
-        <v>0</v>
+        <v>13.100000000000001</v>
       </c>
       <c r="J4" s="1">
-        <v>0</v>
+        <v>982.80000000000007</v>
       </c>
       <c r="K4" s="1">
-        <v>0</v>
+        <v>72.899999999999991</v>
       </c>
       <c r="L4" s="1">
-        <v>0</v>
+        <v>41.7</v>
       </c>
       <c r="M4" s="1">
-        <v>0</v>
+        <v>2.1</v>
       </c>
       <c r="N4" s="1">
-        <v>0</v>
+        <v>0.79999999999999993</v>
       </c>
       <c r="O4" s="1">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="P4" s="1">
         <v>0</v>
       </c>
       <c r="Q4" s="1">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="R4" s="1">
         <v>0</v>
       </c>
       <c r="S4" s="1">
-        <v>0</v>
+        <v>863.7</v>
       </c>
       <c r="T4" s="1">
-        <v>0</v>
+        <v>3140.3999999999996</v>
       </c>
       <c r="U4" s="1">
-        <v>0</v>
+        <v>2983.7</v>
       </c>
       <c r="V4" s="1">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="W4" s="1">
-        <v>0</v>
+        <v>73.699999999999989</v>
       </c>
       <c r="X4" s="1">
         <v>0</v>
       </c>
       <c r="Y4" s="1">
-        <v>0</v>
+        <v>94.7</v>
       </c>
       <c r="Z4" s="1">
-        <v>0</v>
+        <v>69.2</v>
       </c>
       <c r="AA4" s="1">
         <v>0</v>
@@ -14290,13 +14294,13 @@
         <v>0</v>
       </c>
       <c r="AC4" s="1">
-        <v>0</v>
+        <v>25.500000000000004</v>
       </c>
       <c r="AD4" s="1">
-        <v>0</v>
+        <v>2.9000000000000004</v>
       </c>
       <c r="AE4" s="1">
-        <v>0</v>
+        <v>2.9000000000000004</v>
       </c>
       <c r="AF4" s="1">
         <v>0</v>
@@ -14305,13 +14309,13 @@
         <v>0</v>
       </c>
       <c r="AH4" s="1">
-        <v>0</v>
+        <v>1015.5000000000001</v>
       </c>
       <c r="AI4" s="1">
-        <v>0</v>
+        <v>3237.9999999999995</v>
       </c>
       <c r="AJ4" s="1">
-        <v>0</v>
+        <v>4253.4999999999991</v>
       </c>
       <c r="AK4" s="2">
         <v>2022</v>
@@ -14352,7 +14356,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="1">
-        <v>0</v>
+        <v>3.8</v>
       </c>
       <c r="K5" s="1">
         <v>0</v>
@@ -14361,13 +14365,13 @@
         <v>0</v>
       </c>
       <c r="M5" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="N5" s="1">
         <v>0</v>
       </c>
       <c r="O5" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P5" s="1">
         <v>0</v>
@@ -14379,16 +14383,16 @@
         <v>0</v>
       </c>
       <c r="S5" s="1">
-        <v>0</v>
+        <v>2.8</v>
       </c>
       <c r="T5" s="1">
-        <v>0</v>
+        <v>22.2</v>
       </c>
       <c r="U5" s="1">
         <v>0</v>
       </c>
       <c r="V5" s="1">
-        <v>0</v>
+        <v>22.2</v>
       </c>
       <c r="W5" s="1">
         <v>0</v>
@@ -14397,10 +14401,10 @@
         <v>0</v>
       </c>
       <c r="Y5" s="1">
-        <v>0</v>
+        <v>767.3</v>
       </c>
       <c r="Z5" s="1">
-        <v>0</v>
+        <v>21.5</v>
       </c>
       <c r="AA5" s="1">
         <v>0</v>
@@ -14409,28 +14413,28 @@
         <v>0</v>
       </c>
       <c r="AC5" s="1">
-        <v>0</v>
+        <v>745.8</v>
       </c>
       <c r="AD5" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AE5" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AF5" s="1">
         <v>0</v>
       </c>
       <c r="AG5" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AH5" s="1">
-        <v>0</v>
+        <v>3.8</v>
       </c>
       <c r="AI5" s="1">
-        <v>0</v>
+        <v>798.5</v>
       </c>
       <c r="AJ5" s="1">
-        <v>0</v>
+        <v>802.3</v>
       </c>
       <c r="AK5" s="2">
         <v>2022</v>
@@ -14447,109 +14451,109 @@
         <v>38</v>
       </c>
       <c r="B6" s="1">
-        <v>0</v>
+        <v>743.2</v>
       </c>
       <c r="C6" s="1">
-        <v>0</v>
+        <v>91.1</v>
       </c>
       <c r="D6" s="1">
-        <v>0</v>
+        <v>84.9</v>
       </c>
       <c r="E6" s="1">
-        <v>0</v>
+        <v>4.8</v>
       </c>
       <c r="F6" s="1">
-        <v>0</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="G6" s="1">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="H6" s="1">
-        <v>0</v>
+        <v>100.5</v>
       </c>
       <c r="I6" s="1">
-        <v>0</v>
+        <v>455.90000000000003</v>
       </c>
       <c r="J6" s="1">
-        <v>0</v>
+        <v>353</v>
       </c>
       <c r="K6" s="1">
-        <v>0</v>
+        <v>185.29999999999998</v>
       </c>
       <c r="L6" s="1">
-        <v>0</v>
+        <v>85.199999999999989</v>
       </c>
       <c r="M6" s="1">
-        <v>0</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="N6" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O6" s="1">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="P6" s="1">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="Q6" s="1">
-        <v>0</v>
+        <v>12.2</v>
       </c>
       <c r="R6" s="1">
-        <v>0</v>
+        <v>46.9</v>
       </c>
       <c r="S6" s="1">
         <v>0</v>
       </c>
       <c r="T6" s="1">
-        <v>0</v>
+        <v>435.2</v>
       </c>
       <c r="U6" s="1">
-        <v>0</v>
+        <v>300.59999999999997</v>
       </c>
       <c r="V6" s="1">
-        <v>0</v>
+        <v>49.3</v>
       </c>
       <c r="W6" s="1">
-        <v>0</v>
+        <v>85.300000000000011</v>
       </c>
       <c r="X6" s="1">
         <v>0</v>
       </c>
       <c r="Y6" s="1">
-        <v>0</v>
+        <v>52.099999999999994</v>
       </c>
       <c r="Z6" s="1">
-        <v>0</v>
+        <v>9.1</v>
       </c>
       <c r="AA6" s="1">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="AB6" s="1">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AC6" s="1">
-        <v>0</v>
+        <v>41.699999999999996</v>
       </c>
       <c r="AD6" s="1">
-        <v>0</v>
+        <v>9056</v>
       </c>
       <c r="AE6" s="1">
-        <v>0</v>
+        <v>153.4</v>
       </c>
       <c r="AF6" s="1">
-        <v>0</v>
+        <v>1208.2</v>
       </c>
       <c r="AG6" s="1">
-        <v>0</v>
+        <v>7694.4</v>
       </c>
       <c r="AH6" s="1">
-        <v>0</v>
+        <v>1096.2</v>
       </c>
       <c r="AI6" s="1">
-        <v>0</v>
+        <v>9543.2999999999993</v>
       </c>
       <c r="AJ6" s="1">
-        <v>0</v>
+        <v>10639.5</v>
       </c>
       <c r="AK6" s="2">
         <v>2022</v>
@@ -14566,46 +14570,46 @@
         <v>34</v>
       </c>
       <c r="B7" s="1">
-        <v>0</v>
+        <v>179.79999999999998</v>
       </c>
       <c r="C7" s="1">
         <v>0</v>
       </c>
       <c r="D7" s="1">
-        <v>0</v>
+        <v>84.9</v>
       </c>
       <c r="E7" s="1">
-        <v>0</v>
+        <v>4.8</v>
       </c>
       <c r="F7" s="1">
-        <v>0</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="G7" s="1">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="H7" s="1">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="I7" s="1">
-        <v>0</v>
+        <v>9.1</v>
       </c>
       <c r="J7" s="1">
-        <v>0</v>
+        <v>237.60000000000002</v>
       </c>
       <c r="K7" s="1">
-        <v>0</v>
+        <v>169.2</v>
       </c>
       <c r="L7" s="1">
-        <v>0</v>
+        <v>63.8</v>
       </c>
       <c r="M7" s="1">
-        <v>0</v>
+        <v>3.3</v>
       </c>
       <c r="N7" s="1">
         <v>0</v>
       </c>
       <c r="O7" s="1">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="P7" s="1">
         <v>0</v>
@@ -14620,40 +14624,40 @@
         <v>0</v>
       </c>
       <c r="T7" s="1">
-        <v>0</v>
+        <v>286.79999999999995</v>
       </c>
       <c r="U7" s="1">
-        <v>0</v>
+        <v>278.39999999999998</v>
       </c>
       <c r="V7" s="1">
         <v>0</v>
       </c>
       <c r="W7" s="1">
-        <v>0</v>
+        <v>8.4</v>
       </c>
       <c r="X7" s="1">
         <v>0</v>
       </c>
       <c r="Y7" s="1">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="Z7" s="1">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="AA7" s="1">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="AB7" s="1">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="AC7" s="1">
-        <v>0</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="AD7" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AE7" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AF7" s="1">
         <v>0</v>
@@ -14662,13 +14666,13 @@
         <v>0</v>
       </c>
       <c r="AH7" s="1">
-        <v>0</v>
+        <v>417.4</v>
       </c>
       <c r="AI7" s="1">
-        <v>0</v>
+        <v>297.29999999999995</v>
       </c>
       <c r="AJ7" s="1">
-        <v>0</v>
+        <v>714.69999999999993</v>
       </c>
       <c r="AK7" s="2">
         <v>2022</v>
@@ -14685,10 +14689,10 @@
         <v>39</v>
       </c>
       <c r="B8" s="1">
-        <v>0</v>
+        <v>563.4</v>
       </c>
       <c r="C8" s="1">
-        <v>0</v>
+        <v>91.1</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
@@ -14703,61 +14707,61 @@
         <v>0</v>
       </c>
       <c r="H8" s="1">
-        <v>0</v>
+        <v>25.5</v>
       </c>
       <c r="I8" s="1">
-        <v>0</v>
+        <v>446.8</v>
       </c>
       <c r="J8" s="1">
-        <v>0</v>
+        <v>115.4</v>
       </c>
       <c r="K8" s="1">
-        <v>0</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="L8" s="1">
-        <v>0</v>
+        <v>21.4</v>
       </c>
       <c r="M8" s="1">
-        <v>0</v>
+        <v>14.3</v>
       </c>
       <c r="N8" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O8" s="1">
         <v>0</v>
       </c>
       <c r="P8" s="1">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="Q8" s="1">
-        <v>0</v>
+        <v>12.2</v>
       </c>
       <c r="R8" s="1">
-        <v>0</v>
+        <v>46.9</v>
       </c>
       <c r="S8" s="1">
         <v>0</v>
       </c>
       <c r="T8" s="1">
-        <v>0</v>
+        <v>148.4</v>
       </c>
       <c r="U8" s="1">
-        <v>0</v>
+        <v>22.2</v>
       </c>
       <c r="V8" s="1">
-        <v>0</v>
+        <v>49.3</v>
       </c>
       <c r="W8" s="1">
-        <v>0</v>
+        <v>76.900000000000006</v>
       </c>
       <c r="X8" s="1">
         <v>0</v>
       </c>
       <c r="Y8" s="1">
-        <v>0</v>
+        <v>44.599999999999994</v>
       </c>
       <c r="Z8" s="1">
-        <v>0</v>
+        <v>7.3</v>
       </c>
       <c r="AA8" s="1">
         <v>0</v>
@@ -14766,28 +14770,28 @@
         <v>0</v>
       </c>
       <c r="AC8" s="1">
-        <v>0</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="AD8" s="1">
-        <v>0</v>
+        <v>9053</v>
       </c>
       <c r="AE8" s="1">
-        <v>0</v>
+        <v>150.4</v>
       </c>
       <c r="AF8" s="1">
-        <v>0</v>
+        <v>1208.2</v>
       </c>
       <c r="AG8" s="1">
-        <v>0</v>
+        <v>7694.4</v>
       </c>
       <c r="AH8" s="1">
-        <v>0</v>
+        <v>678.8</v>
       </c>
       <c r="AI8" s="1">
-        <v>0</v>
+        <v>9246</v>
       </c>
       <c r="AJ8" s="1">
-        <v>0</v>
+        <v>9924.7999999999993</v>
       </c>
       <c r="AK8" s="2">
         <v>2022</v>
@@ -14804,109 +14808,109 @@
         <v>40</v>
       </c>
       <c r="B9" s="1">
-        <v>0</v>
+        <v>106.9</v>
       </c>
       <c r="C9" s="1">
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="D9" s="1">
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="E9" s="1">
-        <v>0</v>
+        <v>3.1</v>
       </c>
       <c r="F9" s="1">
-        <v>0</v>
+        <v>2.1</v>
       </c>
       <c r="G9" s="1">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H9" s="1">
-        <v>0</v>
+        <v>21.3</v>
       </c>
       <c r="I9" s="1">
-        <v>0</v>
+        <v>72.900000000000006</v>
       </c>
       <c r="J9" s="1">
-        <v>0</v>
+        <v>664.8</v>
       </c>
       <c r="K9" s="1">
-        <v>0</v>
+        <v>29.1</v>
       </c>
       <c r="L9" s="1">
-        <v>0</v>
+        <v>67.099999999999994</v>
       </c>
       <c r="M9" s="1">
-        <v>0</v>
+        <v>114.8</v>
       </c>
       <c r="N9" s="1">
-        <v>0</v>
+        <v>19.7</v>
       </c>
       <c r="O9" s="1">
-        <v>0</v>
+        <v>37.9</v>
       </c>
       <c r="P9" s="1">
-        <v>0</v>
+        <v>95.7</v>
       </c>
       <c r="Q9" s="1">
-        <v>0</v>
+        <v>10.4</v>
       </c>
       <c r="R9" s="1">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="S9" s="1">
-        <v>0</v>
+        <v>287.39999999999998</v>
       </c>
       <c r="T9" s="1">
-        <v>0</v>
+        <v>578.20000000000005</v>
       </c>
       <c r="U9" s="1">
-        <v>0</v>
+        <v>261.8</v>
       </c>
       <c r="V9" s="1">
-        <v>0</v>
+        <v>13.1</v>
       </c>
       <c r="W9" s="1">
-        <v>0</v>
+        <v>264.5</v>
       </c>
       <c r="X9" s="1">
-        <v>0</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="Y9" s="1">
-        <v>0</v>
+        <v>648.70000000000005</v>
       </c>
       <c r="Z9" s="1">
-        <v>0</v>
+        <v>470.3</v>
       </c>
       <c r="AA9" s="1">
-        <v>0</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="AB9" s="1">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AC9" s="1">
-        <v>0</v>
+        <v>167.6</v>
       </c>
       <c r="AD9" s="1">
-        <v>0</v>
+        <v>901.3</v>
       </c>
       <c r="AE9" s="1">
-        <v>0</v>
+        <v>721.3</v>
       </c>
       <c r="AF9" s="1">
-        <v>0</v>
+        <v>110.3</v>
       </c>
       <c r="AG9" s="1">
-        <v>0</v>
+        <v>69.7</v>
       </c>
       <c r="AH9" s="1">
-        <v>0</v>
+        <v>771.69999999999993</v>
       </c>
       <c r="AI9" s="1">
-        <v>0</v>
+        <v>2128.1999999999998</v>
       </c>
       <c r="AJ9" s="1">
-        <v>0</v>
+        <v>2899.8999999999996</v>
       </c>
       <c r="AK9" s="2">
         <v>2022</v>
@@ -14923,13 +14927,13 @@
         <v>41</v>
       </c>
       <c r="B10" s="1">
-        <v>0</v>
+        <v>7.9000000000000012</v>
       </c>
       <c r="C10" s="1">
         <v>0</v>
       </c>
       <c r="D10" s="1">
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="E10" s="1">
         <v>0</v>
@@ -14938,16 +14942,16 @@
         <v>0</v>
       </c>
       <c r="G10" s="1">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H10" s="1">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="I10" s="1">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="J10" s="1">
-        <v>0</v>
+        <v>246.7</v>
       </c>
       <c r="K10" s="1">
         <v>0</v>
@@ -14956,76 +14960,76 @@
         <v>0</v>
       </c>
       <c r="M10" s="1">
-        <v>0</v>
+        <v>3.1</v>
       </c>
       <c r="N10" s="1">
         <v>0</v>
       </c>
       <c r="O10" s="1">
-        <v>0</v>
+        <v>12.3</v>
       </c>
       <c r="P10" s="1">
-        <v>0</v>
+        <v>48.2</v>
       </c>
       <c r="Q10" s="1">
-        <v>0</v>
+        <v>7.9</v>
       </c>
       <c r="R10" s="1">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="S10" s="1">
-        <v>0</v>
+        <v>172.5</v>
       </c>
       <c r="T10" s="1">
-        <v>0</v>
+        <v>477.1</v>
       </c>
       <c r="U10" s="1">
-        <v>0</v>
+        <v>180.1</v>
       </c>
       <c r="V10" s="1">
-        <v>0</v>
+        <v>13.1</v>
       </c>
       <c r="W10" s="1">
-        <v>0</v>
+        <v>247.9</v>
       </c>
       <c r="X10" s="1">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="Y10" s="1">
-        <v>0</v>
+        <v>628.69999999999993</v>
       </c>
       <c r="Z10" s="1">
-        <v>0</v>
+        <v>451.4</v>
       </c>
       <c r="AA10" s="1">
-        <v>0</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="AB10" s="1">
         <v>0</v>
       </c>
       <c r="AC10" s="1">
-        <v>0</v>
+        <v>167.6</v>
       </c>
       <c r="AD10" s="1">
-        <v>0</v>
+        <v>361</v>
       </c>
       <c r="AE10" s="1">
-        <v>0</v>
+        <v>313.8</v>
       </c>
       <c r="AF10" s="1">
-        <v>0</v>
+        <v>25.3</v>
       </c>
       <c r="AG10" s="1">
-        <v>0</v>
+        <v>21.9</v>
       </c>
       <c r="AH10" s="1">
-        <v>0</v>
+        <v>254.6</v>
       </c>
       <c r="AI10" s="1">
-        <v>0</v>
+        <v>1466.8</v>
       </c>
       <c r="AJ10" s="1">
-        <v>0</v>
+        <v>1721.3999999999999</v>
       </c>
       <c r="AK10" s="2">
         <v>2022</v>
@@ -15066,7 +15070,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="1">
-        <v>0</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="K11" s="1">
         <v>0</v>
@@ -15081,10 +15085,10 @@
         <v>0</v>
       </c>
       <c r="O11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P11" s="1">
-        <v>0</v>
+        <v>7.8</v>
       </c>
       <c r="Q11" s="1">
         <v>0</v>
@@ -15096,7 +15100,7 @@
         <v>0</v>
       </c>
       <c r="T11" s="1">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="U11" s="1">
         <v>0</v>
@@ -15108,43 +15112,43 @@
         <v>0</v>
       </c>
       <c r="X11" s="1">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="Y11" s="1">
-        <v>0</v>
+        <v>12.799999999999999</v>
       </c>
       <c r="Z11" s="1">
-        <v>0</v>
+        <v>11.7</v>
       </c>
       <c r="AA11" s="1">
         <v>0</v>
       </c>
       <c r="AB11" s="1">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AC11" s="1">
         <v>0</v>
       </c>
       <c r="AD11" s="1">
-        <v>0</v>
+        <v>540.29999999999995</v>
       </c>
       <c r="AE11" s="1">
-        <v>0</v>
+        <v>407.5</v>
       </c>
       <c r="AF11" s="1">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="AG11" s="1">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="AH11" s="1">
-        <v>0</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="AI11" s="1">
-        <v>0</v>
+        <v>555.79999999999995</v>
       </c>
       <c r="AJ11" s="1">
-        <v>0</v>
+        <v>564.59999999999991</v>
       </c>
       <c r="AK11" s="2">
         <v>2022</v>
@@ -15161,79 +15165,79 @@
         <v>43</v>
       </c>
       <c r="B12" s="1">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="C12" s="1">
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
       </c>
       <c r="E12" s="1">
-        <v>0</v>
+        <v>3.1</v>
       </c>
       <c r="F12" s="1">
-        <v>0</v>
+        <v>2.1</v>
       </c>
       <c r="G12" s="1">
         <v>0</v>
       </c>
       <c r="H12" s="1">
-        <v>0</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="I12" s="1">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="J12" s="1">
-        <v>0</v>
+        <v>409.5</v>
       </c>
       <c r="K12" s="1">
-        <v>0</v>
+        <v>29.1</v>
       </c>
       <c r="L12" s="1">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="M12" s="1">
-        <v>0</v>
+        <v>111.7</v>
       </c>
       <c r="N12" s="1">
-        <v>0</v>
+        <v>19.7</v>
       </c>
       <c r="O12" s="1">
-        <v>0</v>
+        <v>24.7</v>
       </c>
       <c r="P12" s="1">
-        <v>0</v>
+        <v>39.9</v>
       </c>
       <c r="Q12" s="1">
-        <v>0</v>
+        <v>2.6</v>
       </c>
       <c r="R12" s="1">
         <v>0</v>
       </c>
       <c r="S12" s="1">
-        <v>0</v>
+        <v>114.8</v>
       </c>
       <c r="T12" s="1">
-        <v>0</v>
+        <v>98.3</v>
       </c>
       <c r="U12" s="1">
-        <v>0</v>
+        <v>81.7</v>
       </c>
       <c r="V12" s="1">
         <v>0</v>
       </c>
       <c r="W12" s="1">
-        <v>0</v>
+        <v>16.5</v>
       </c>
       <c r="X12" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="Y12" s="1">
-        <v>0</v>
+        <v>7.3999999999999995</v>
       </c>
       <c r="Z12" s="1">
-        <v>0</v>
+        <v>7.3999999999999995</v>
       </c>
       <c r="AA12" s="1">
         <v>0</v>
@@ -15257,13 +15261,13 @@
         <v>0</v>
       </c>
       <c r="AH12" s="1">
-        <v>0</v>
+        <v>508.5</v>
       </c>
       <c r="AI12" s="1">
-        <v>0</v>
+        <v>105.7</v>
       </c>
       <c r="AJ12" s="1">
-        <v>0</v>
+        <v>614.20000000000005</v>
       </c>
       <c r="AK12" s="2">
         <v>2022</v>
@@ -15280,7 +15284,7 @@
         <v>44</v>
       </c>
       <c r="B13" s="1">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="C13" s="1">
         <v>0</v>
@@ -15298,10 +15302,10 @@
         <v>0</v>
       </c>
       <c r="H13" s="1">
-        <v>0</v>
+        <v>30.7</v>
       </c>
       <c r="I13" s="1">
-        <v>0</v>
+        <v>20.3</v>
       </c>
       <c r="J13" s="1">
         <v>0</v>
@@ -15334,16 +15338,16 @@
         <v>0</v>
       </c>
       <c r="T13" s="1">
-        <v>0</v>
+        <v>59.9</v>
       </c>
       <c r="U13" s="1">
-        <v>0</v>
+        <v>58.4</v>
       </c>
       <c r="V13" s="1">
         <v>0</v>
       </c>
       <c r="W13" s="1">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="X13" s="1">
         <v>0</v>
@@ -15376,13 +15380,13 @@
         <v>0</v>
       </c>
       <c r="AH13" s="1">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="AI13" s="1">
-        <v>0</v>
+        <v>59.9</v>
       </c>
       <c r="AJ13" s="1">
-        <v>0</v>
+        <v>110.9</v>
       </c>
       <c r="AK13" s="2">
         <v>2022</v>
@@ -15453,25 +15457,25 @@
         <v>0</v>
       </c>
       <c r="T14" s="1">
-        <v>0</v>
+        <v>52.2</v>
       </c>
       <c r="U14" s="1">
-        <v>0</v>
+        <v>13.3</v>
       </c>
       <c r="V14" s="1">
         <v>0</v>
       </c>
       <c r="W14" s="1">
-        <v>0</v>
+        <v>37.4</v>
       </c>
       <c r="X14" s="1">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="Y14" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Z14" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA14" s="1">
         <v>0</v>
@@ -15483,7 +15487,7 @@
         <v>0</v>
       </c>
       <c r="AD14" s="1">
-        <v>0</v>
+        <v>5.2</v>
       </c>
       <c r="AE14" s="1">
         <v>0</v>
@@ -15492,16 +15496,16 @@
         <v>0</v>
       </c>
       <c r="AG14" s="1">
-        <v>0</v>
+        <v>5.2</v>
       </c>
       <c r="AH14" s="1">
         <v>0</v>
       </c>
       <c r="AI14" s="1">
-        <v>0</v>
+        <v>60.400000000000006</v>
       </c>
       <c r="AJ14" s="1">
-        <v>0</v>
+        <v>60.400000000000006</v>
       </c>
       <c r="AK14" s="2">
         <v>2022</v>
@@ -15542,7 +15546,7 @@
         <v>0</v>
       </c>
       <c r="J15" s="1">
-        <v>0</v>
+        <v>37.800000000000004</v>
       </c>
       <c r="K15" s="1">
         <v>0</v>
@@ -15551,7 +15555,7 @@
         <v>0</v>
       </c>
       <c r="M15" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="N15" s="1">
         <v>0</v>
@@ -15569,13 +15573,13 @@
         <v>0</v>
       </c>
       <c r="S15" s="1">
-        <v>0</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="T15" s="1">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="U15" s="1">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="V15" s="1">
         <v>0</v>
@@ -15614,13 +15618,13 @@
         <v>0</v>
       </c>
       <c r="AH15" s="1">
-        <v>0</v>
+        <v>37.800000000000004</v>
       </c>
       <c r="AI15" s="1">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="AJ15" s="1">
-        <v>0</v>
+        <v>38.500000000000007</v>
       </c>
       <c r="AK15" s="2">
         <v>2022</v>
@@ -15637,109 +15641,109 @@
         <v>47</v>
       </c>
       <c r="B16" s="1">
-        <v>0</v>
+        <v>5219.1000000000004</v>
       </c>
       <c r="C16" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="D16" s="1">
-        <v>0</v>
+        <v>1480.3</v>
       </c>
       <c r="E16" s="1">
-        <v>0</v>
+        <v>155.30000000000001</v>
       </c>
       <c r="F16" s="1">
-        <v>0</v>
+        <v>9.6</v>
       </c>
       <c r="G16" s="1">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="H16" s="1">
-        <v>0</v>
+        <v>1349.8</v>
       </c>
       <c r="I16" s="1">
-        <v>0</v>
+        <v>2132.9</v>
       </c>
       <c r="J16" s="1">
-        <v>0</v>
+        <v>10977.900000000001</v>
       </c>
       <c r="K16" s="1">
-        <v>0</v>
+        <v>3069.8</v>
       </c>
       <c r="L16" s="1">
-        <v>0</v>
+        <v>2787.4</v>
       </c>
       <c r="M16" s="1">
-        <v>0</v>
+        <v>540.4</v>
       </c>
       <c r="N16" s="1">
-        <v>0</v>
+        <v>29.1</v>
       </c>
       <c r="O16" s="1">
-        <v>0</v>
+        <v>72.2</v>
       </c>
       <c r="P16" s="1">
-        <v>0</v>
+        <v>160.5</v>
       </c>
       <c r="Q16" s="1">
-        <v>0</v>
+        <v>83.9</v>
       </c>
       <c r="R16" s="1">
-        <v>0</v>
+        <v>949.1</v>
       </c>
       <c r="S16" s="1">
-        <v>0</v>
+        <v>3285.5</v>
       </c>
       <c r="T16" s="1">
-        <v>0</v>
+        <v>69269.099999999991</v>
       </c>
       <c r="U16" s="1">
-        <v>0</v>
+        <v>44614.7</v>
       </c>
       <c r="V16" s="1">
-        <v>0</v>
+        <v>11159.3</v>
       </c>
       <c r="W16" s="1">
-        <v>0</v>
+        <v>12990.7</v>
       </c>
       <c r="X16" s="1">
-        <v>0</v>
+        <v>504.4</v>
       </c>
       <c r="Y16" s="1">
-        <v>0</v>
+        <v>13161.100000000002</v>
       </c>
       <c r="Z16" s="1">
-        <v>0</v>
+        <v>8917.6</v>
       </c>
       <c r="AA16" s="1">
-        <v>0</v>
+        <v>40.200000000000003</v>
       </c>
       <c r="AB16" s="1">
-        <v>0</v>
+        <v>7.1</v>
       </c>
       <c r="AC16" s="1">
-        <v>0</v>
+        <v>4196.2</v>
       </c>
       <c r="AD16" s="1">
-        <v>0</v>
+        <v>27770.1</v>
       </c>
       <c r="AE16" s="1">
-        <v>0</v>
+        <v>19254.3</v>
       </c>
       <c r="AF16" s="1">
-        <v>0</v>
+        <v>2685.3</v>
       </c>
       <c r="AG16" s="1">
-        <v>0</v>
+        <v>5830.5</v>
       </c>
       <c r="AH16" s="1">
-        <v>0</v>
+        <v>16197.000000000002</v>
       </c>
       <c r="AI16" s="1">
-        <v>0</v>
+        <v>110200.29999999999</v>
       </c>
       <c r="AJ16" s="1">
-        <v>0</v>
+        <v>126397.29999999999</v>
       </c>
       <c r="AK16" s="2">
         <v>2022</v>
@@ -15756,37 +15760,37 @@
         <v>48</v>
       </c>
       <c r="B17" s="1">
-        <v>0</v>
+        <v>8928.2000000000007</v>
       </c>
       <c r="C17" s="1">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="D17" s="1">
-        <v>0</v>
+        <v>1705.4</v>
       </c>
       <c r="E17" s="1">
-        <v>0</v>
+        <v>28.8</v>
       </c>
       <c r="F17" s="1">
-        <v>0</v>
+        <v>19.8</v>
       </c>
       <c r="G17" s="1">
-        <v>0</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="H17" s="1">
-        <v>0</v>
+        <v>2790.1</v>
       </c>
       <c r="I17" s="1">
-        <v>0</v>
+        <v>4006.5</v>
       </c>
       <c r="J17" s="1">
-        <v>0</v>
+        <v>14491.599999999999</v>
       </c>
       <c r="K17" s="1">
-        <v>0</v>
+        <v>3759.7</v>
       </c>
       <c r="L17" s="1">
-        <v>0</v>
+        <v>3234.1</v>
       </c>
       <c r="M17" s="1">
         <v>0</v>
@@ -15801,34 +15805,34 @@
         <v>0</v>
       </c>
       <c r="Q17" s="1">
-        <v>0</v>
+        <v>9.1</v>
       </c>
       <c r="R17" s="1">
         <v>0</v>
       </c>
       <c r="S17" s="1">
-        <v>0</v>
+        <v>7488.7</v>
       </c>
       <c r="T17" s="1">
-        <v>0</v>
+        <v>72624.3</v>
       </c>
       <c r="U17" s="1">
-        <v>0</v>
+        <v>41538.300000000003</v>
       </c>
       <c r="V17" s="1">
-        <v>0</v>
+        <v>13347.1</v>
       </c>
       <c r="W17" s="1">
-        <v>0</v>
+        <v>17420.400000000001</v>
       </c>
       <c r="X17" s="1">
-        <v>0</v>
+        <v>318.5</v>
       </c>
       <c r="Y17" s="1">
-        <v>0</v>
+        <v>12363.7</v>
       </c>
       <c r="Z17" s="1">
-        <v>0</v>
+        <v>7868</v>
       </c>
       <c r="AA17" s="1">
         <v>0</v>
@@ -15837,28 +15841,28 @@
         <v>0</v>
       </c>
       <c r="AC17" s="1">
-        <v>0</v>
+        <v>4495.7</v>
       </c>
       <c r="AD17" s="1">
-        <v>0</v>
+        <v>45130.399999999994</v>
       </c>
       <c r="AE17" s="1">
-        <v>0</v>
+        <v>20804.3</v>
       </c>
       <c r="AF17" s="1">
-        <v>0</v>
+        <v>2498</v>
       </c>
       <c r="AG17" s="1">
-        <v>0</v>
+        <v>21828.1</v>
       </c>
       <c r="AH17" s="1">
-        <v>0</v>
+        <v>23419.8</v>
       </c>
       <c r="AI17" s="1">
-        <v>0</v>
+        <v>130118.39999999999</v>
       </c>
       <c r="AJ17" s="1">
-        <v>0</v>
+        <v>153538.19999999998</v>
       </c>
       <c r="AK17" s="2">
         <v>2022</v>
@@ -15875,7 +15879,7 @@
         <v>49</v>
       </c>
       <c r="B18" s="1">
-        <v>0</v>
+        <v>166.1</v>
       </c>
       <c r="C18" s="1">
         <v>0</v>
@@ -15893,25 +15897,25 @@
         <v>0</v>
       </c>
       <c r="H18" s="1">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="I18" s="1">
-        <v>0</v>
+        <v>112.1</v>
       </c>
       <c r="J18" s="1">
-        <v>0</v>
+        <v>311.7</v>
       </c>
       <c r="K18" s="1">
-        <v>0</v>
+        <v>23.6</v>
       </c>
       <c r="L18" s="1">
-        <v>0</v>
+        <v>46.4</v>
       </c>
       <c r="M18" s="1">
         <v>0</v>
       </c>
       <c r="N18" s="1">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="O18" s="1">
         <v>0</v>
@@ -15926,28 +15930,28 @@
         <v>0</v>
       </c>
       <c r="S18" s="1">
-        <v>0</v>
+        <v>240.9</v>
       </c>
       <c r="T18" s="1">
-        <v>0</v>
+        <v>1725.5</v>
       </c>
       <c r="U18" s="1">
-        <v>0</v>
+        <v>174.9</v>
       </c>
       <c r="V18" s="1">
-        <v>0</v>
+        <v>340.3</v>
       </c>
       <c r="W18" s="1">
-        <v>0</v>
+        <v>1174.5</v>
       </c>
       <c r="X18" s="1">
-        <v>0</v>
+        <v>35.799999999999997</v>
       </c>
       <c r="Y18" s="1">
-        <v>0</v>
+        <v>712</v>
       </c>
       <c r="Z18" s="1">
-        <v>0</v>
+        <v>669.7</v>
       </c>
       <c r="AA18" s="1">
         <v>0</v>
@@ -15956,13 +15960,13 @@
         <v>0</v>
       </c>
       <c r="AC18" s="1">
-        <v>0</v>
+        <v>42.3</v>
       </c>
       <c r="AD18" s="1">
-        <v>0</v>
+        <v>52.9</v>
       </c>
       <c r="AE18" s="1">
-        <v>0</v>
+        <v>52.9</v>
       </c>
       <c r="AF18" s="1">
         <v>0</v>
@@ -15971,13 +15975,13 @@
         <v>0</v>
       </c>
       <c r="AH18" s="1">
-        <v>0</v>
+        <v>477.79999999999995</v>
       </c>
       <c r="AI18" s="1">
-        <v>0</v>
+        <v>2490.4</v>
       </c>
       <c r="AJ18" s="1">
-        <v>0</v>
+        <v>2968.2</v>
       </c>
       <c r="AK18" s="2">
         <v>2022</v>
@@ -16048,13 +16052,13 @@
         <v>0</v>
       </c>
       <c r="T19" s="1">
-        <v>0</v>
+        <v>74.3</v>
       </c>
       <c r="U19" s="1">
         <v>0</v>
       </c>
       <c r="V19" s="1">
-        <v>0</v>
+        <v>74.3</v>
       </c>
       <c r="W19" s="1">
         <v>0</v>
@@ -16078,25 +16082,25 @@
         <v>0</v>
       </c>
       <c r="AD19" s="1">
-        <v>0</v>
+        <v>1101.3</v>
       </c>
       <c r="AE19" s="1">
-        <v>0</v>
+        <v>241.2</v>
       </c>
       <c r="AF19" s="1">
         <v>0</v>
       </c>
       <c r="AG19" s="1">
-        <v>0</v>
+        <v>860.1</v>
       </c>
       <c r="AH19" s="1">
         <v>0</v>
       </c>
       <c r="AI19" s="1">
-        <v>0</v>
+        <v>1175.5999999999999</v>
       </c>
       <c r="AJ19" s="1">
-        <v>0</v>
+        <v>1175.5999999999999</v>
       </c>
       <c r="AK19" s="2">
         <v>2022</v>
@@ -16197,25 +16201,25 @@
         <v>0</v>
       </c>
       <c r="AD20" s="1">
-        <v>0</v>
+        <v>83.3</v>
       </c>
       <c r="AE20" s="1">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="AF20" s="1">
         <v>0</v>
       </c>
       <c r="AG20" s="1">
-        <v>0</v>
+        <v>82.1</v>
       </c>
       <c r="AH20" s="1">
         <v>0</v>
       </c>
       <c r="AI20" s="1">
-        <v>0</v>
+        <v>83.3</v>
       </c>
       <c r="AJ20" s="1">
-        <v>0</v>
+        <v>83.3</v>
       </c>
       <c r="AK20" s="2">
         <v>2022</v>
@@ -16316,25 +16320,25 @@
         <v>0</v>
       </c>
       <c r="AD21" s="1">
-        <v>0</v>
+        <v>12.399999999999999</v>
       </c>
       <c r="AE21" s="1">
-        <v>0</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="AF21" s="1">
         <v>0</v>
       </c>
       <c r="AG21" s="1">
-        <v>0</v>
+        <v>3.7</v>
       </c>
       <c r="AH21" s="1">
         <v>0</v>
       </c>
       <c r="AI21" s="1">
-        <v>0</v>
+        <v>12.399999999999999</v>
       </c>
       <c r="AJ21" s="1">
-        <v>0</v>
+        <v>12.399999999999999</v>
       </c>
       <c r="AK21" s="2">
         <v>2022</v>
@@ -16435,25 +16439,25 @@
         <v>0</v>
       </c>
       <c r="AD22" s="1">
-        <v>0</v>
+        <v>496.79999999999995</v>
       </c>
       <c r="AE22" s="1">
-        <v>0</v>
+        <v>372.4</v>
       </c>
       <c r="AF22" s="1">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="AG22" s="1">
-        <v>0</v>
+        <v>122.7</v>
       </c>
       <c r="AH22" s="1">
         <v>0</v>
       </c>
       <c r="AI22" s="1">
-        <v>0</v>
+        <v>496.79999999999995</v>
       </c>
       <c r="AJ22" s="1">
-        <v>0</v>
+        <v>496.79999999999995</v>
       </c>
       <c r="AK22" s="2">
         <v>2022</v>
@@ -16494,7 +16498,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="1">
-        <v>0</v>
+        <v>39.9</v>
       </c>
       <c r="K23" s="1">
         <v>0</v>
@@ -16521,28 +16525,28 @@
         <v>0</v>
       </c>
       <c r="S23" s="1">
-        <v>0</v>
+        <v>39.9</v>
       </c>
       <c r="T23" s="1">
-        <v>0</v>
+        <v>194.29999999999998</v>
       </c>
       <c r="U23" s="1">
         <v>0</v>
       </c>
       <c r="V23" s="1">
-        <v>0</v>
+        <v>48.6</v>
       </c>
       <c r="W23" s="1">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="X23" s="1">
-        <v>0</v>
+        <v>10.7</v>
       </c>
       <c r="Y23" s="1">
-        <v>0</v>
+        <v>606.09999999999991</v>
       </c>
       <c r="Z23" s="1">
-        <v>0</v>
+        <v>298.7</v>
       </c>
       <c r="AA23" s="1">
         <v>0</v>
@@ -16551,28 +16555,28 @@
         <v>0</v>
       </c>
       <c r="AC23" s="1">
-        <v>0</v>
+        <v>307.39999999999998</v>
       </c>
       <c r="AD23" s="1">
-        <v>0</v>
+        <v>8660.6</v>
       </c>
       <c r="AE23" s="1">
-        <v>0</v>
+        <v>3624.8</v>
       </c>
       <c r="AF23" s="1">
-        <v>0</v>
+        <v>475.7</v>
       </c>
       <c r="AG23" s="1">
-        <v>0</v>
+        <v>4560.1000000000004</v>
       </c>
       <c r="AH23" s="1">
-        <v>0</v>
+        <v>39.9</v>
       </c>
       <c r="AI23" s="1">
-        <v>0</v>
+        <v>9461</v>
       </c>
       <c r="AJ23" s="1">
-        <v>0</v>
+        <v>9500.9</v>
       </c>
       <c r="AK23" s="2">
         <v>2022</v>
@@ -16658,7 +16662,7 @@
         <v>0</v>
       </c>
       <c r="Y24" s="1">
-        <v>0</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="Z24" s="1">
         <v>0</v>
@@ -16670,28 +16674,28 @@
         <v>0</v>
       </c>
       <c r="AC24" s="1">
-        <v>0</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="AD24" s="1">
-        <v>0</v>
+        <v>52.900000000000006</v>
       </c>
       <c r="AE24" s="1">
-        <v>0</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="AF24" s="1">
         <v>0</v>
       </c>
       <c r="AG24" s="1">
-        <v>0</v>
+        <v>18.7</v>
       </c>
       <c r="AH24" s="1">
         <v>0</v>
       </c>
       <c r="AI24" s="1">
-        <v>0</v>
+        <v>57.800000000000004</v>
       </c>
       <c r="AJ24" s="1">
-        <v>0</v>
+        <v>57.800000000000004</v>
       </c>
       <c r="AK24" s="2">
         <v>2022</v>
@@ -16708,109 +16712,144 @@
         <v>56</v>
       </c>
       <c r="B25" s="1">
-        <v>0</v>
+        <f>SUM(B2,B5:B6,B9,B13:B24)</f>
+        <v>15267.900000000001</v>
       </c>
       <c r="C25" s="1">
-        <v>0</v>
+        <f t="shared" ref="C25:AJ25" si="0">SUM(C2,C5:C6,C9,C13:C24)</f>
+        <v>544.29999999999995</v>
       </c>
       <c r="D25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3305.4</v>
       </c>
       <c r="E25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>192.00000000000003</v>
       </c>
       <c r="F25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>36.599999999999994</v>
       </c>
       <c r="G25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>20.8</v>
       </c>
       <c r="H25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>4346.3999999999996</v>
       </c>
       <c r="I25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>6822.4000000000005</v>
       </c>
       <c r="J25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>28545.7</v>
       </c>
       <c r="K25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>7191.1</v>
       </c>
       <c r="L25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>6290.9</v>
       </c>
       <c r="M25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>676.59999999999991</v>
       </c>
       <c r="N25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>53.8</v>
       </c>
       <c r="O25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>113.2</v>
       </c>
       <c r="P25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>257.7</v>
       </c>
       <c r="Q25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>116.9</v>
       </c>
       <c r="R25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>998.7</v>
       </c>
       <c r="S25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>12846.8</v>
       </c>
       <c r="T25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>150383.19999999995</v>
       </c>
       <c r="U25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>92045.599999999991</v>
       </c>
       <c r="V25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>25195.799999999996</v>
       </c>
       <c r="W25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>32232.100000000002</v>
       </c>
       <c r="X25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>909.69999999999993</v>
       </c>
       <c r="Y25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>28481.500000000004</v>
       </c>
       <c r="Z25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>18374.800000000003</v>
       </c>
       <c r="AA25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>50.300000000000004</v>
       </c>
       <c r="AB25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>9.1</v>
       </c>
       <c r="AC25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>10047.299999999999</v>
       </c>
       <c r="AD25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>93337.099999999991</v>
       </c>
       <c r="AE25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>45277.599999999991</v>
       </c>
       <c r="AF25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>6979.2</v>
       </c>
       <c r="AG25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>41080.299999999981</v>
       </c>
       <c r="AH25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>43813.600000000006</v>
       </c>
       <c r="AI25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>272201.8</v>
       </c>
       <c r="AJ25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>316015.39999999997</v>
       </c>
       <c r="AK25" s="2">
         <v>2022</v>
@@ -16823,6 +16862,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -16834,8 +16874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37856A1E-82E7-45AE-A2B0-C510B7D63887}">
   <dimension ref="A1:AM36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:Y36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16961,40 +17001,40 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>0</v>
+        <v>53.400000000000006</v>
       </c>
       <c r="C2" s="1">
-        <v>0</v>
+        <v>20.7</v>
       </c>
       <c r="D2" s="1">
-        <v>0</v>
+        <v>32.700000000000003</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
       </c>
       <c r="F2" s="1">
-        <v>0</v>
+        <v>743.2</v>
       </c>
       <c r="G2" s="1">
-        <v>0</v>
+        <v>179.79999999999998</v>
       </c>
       <c r="H2" s="1">
-        <v>0</v>
+        <v>563.4</v>
       </c>
       <c r="I2" s="1">
-        <v>0</v>
+        <v>106.9</v>
       </c>
       <c r="J2" s="1">
-        <v>0</v>
+        <v>7.9000000000000012</v>
       </c>
       <c r="K2" s="1">
         <v>0</v>
       </c>
       <c r="L2" s="1">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="M2" s="1">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="N2" s="1">
         <v>0</v>
@@ -17003,13 +17043,13 @@
         <v>0</v>
       </c>
       <c r="P2" s="1">
-        <v>0</v>
+        <v>5219.1000000000004</v>
       </c>
       <c r="Q2" s="1">
-        <v>0</v>
+        <v>8928.2000000000007</v>
       </c>
       <c r="R2" s="1">
-        <v>0</v>
+        <v>166.1</v>
       </c>
       <c r="S2" s="1">
         <v>0</v>
@@ -17030,7 +17070,8 @@
         <v>0</v>
       </c>
       <c r="Y2" s="1">
-        <v>0</v>
+        <f t="shared" ref="Y2:Y36" si="0">SUM(B2,E2:F2,I2,M2:X2)</f>
+        <v>15267.900000000001</v>
       </c>
       <c r="Z2">
         <v>2022</v>
@@ -17059,16 +17100,16 @@
         <v>0</v>
       </c>
       <c r="F3" s="1">
-        <v>0</v>
+        <v>91.1</v>
       </c>
       <c r="G3" s="1">
         <v>0</v>
       </c>
       <c r="H3" s="1">
-        <v>0</v>
+        <v>91.1</v>
       </c>
       <c r="I3" s="1">
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="J3" s="1">
         <v>0</v>
@@ -17077,7 +17118,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="1">
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="M3" s="1">
         <v>0</v>
@@ -17089,10 +17130,10 @@
         <v>0</v>
       </c>
       <c r="P3" s="1">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="Q3" s="1">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="R3" s="1">
         <v>0</v>
@@ -17116,7 +17157,8 @@
         <v>0</v>
       </c>
       <c r="Y3" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>544.29999999999995</v>
       </c>
       <c r="Z3">
         <v>2022</v>
@@ -17133,31 +17175,31 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>0</v>
+        <v>31.6</v>
       </c>
       <c r="C4" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
       </c>
       <c r="F4" s="1">
-        <v>0</v>
+        <v>84.9</v>
       </c>
       <c r="G4" s="1">
-        <v>0</v>
+        <v>84.9</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
       </c>
       <c r="I4" s="1">
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="J4" s="1">
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="K4" s="1">
         <v>0</v>
@@ -17175,10 +17217,10 @@
         <v>0</v>
       </c>
       <c r="P4" s="1">
-        <v>0</v>
+        <v>1480.3</v>
       </c>
       <c r="Q4" s="1">
-        <v>0</v>
+        <v>1705.4</v>
       </c>
       <c r="R4" s="1">
         <v>0</v>
@@ -17202,7 +17244,8 @@
         <v>0</v>
       </c>
       <c r="Y4" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3305.4</v>
       </c>
       <c r="Z4">
         <v>2022</v>
@@ -17231,16 +17274,16 @@
         <v>0</v>
       </c>
       <c r="F5" s="1">
-        <v>0</v>
+        <v>4.8</v>
       </c>
       <c r="G5" s="1">
-        <v>0</v>
+        <v>4.8</v>
       </c>
       <c r="H5" s="1">
         <v>0</v>
       </c>
       <c r="I5" s="1">
-        <v>0</v>
+        <v>3.1</v>
       </c>
       <c r="J5" s="1">
         <v>0</v>
@@ -17249,7 +17292,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="1">
-        <v>0</v>
+        <v>3.1</v>
       </c>
       <c r="M5" s="1">
         <v>0</v>
@@ -17261,10 +17304,10 @@
         <v>0</v>
       </c>
       <c r="P5" s="1">
-        <v>0</v>
+        <v>155.30000000000001</v>
       </c>
       <c r="Q5" s="1">
-        <v>0</v>
+        <v>28.8</v>
       </c>
       <c r="R5" s="1">
         <v>0</v>
@@ -17288,7 +17331,8 @@
         <v>0</v>
       </c>
       <c r="Y5" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>192.00000000000003</v>
       </c>
       <c r="Z5">
         <v>2022</v>
@@ -17317,16 +17361,16 @@
         <v>0</v>
       </c>
       <c r="F6" s="1">
-        <v>0</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="G6" s="1">
-        <v>0</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="H6" s="1">
         <v>0</v>
       </c>
       <c r="I6" s="1">
-        <v>0</v>
+        <v>2.1</v>
       </c>
       <c r="J6" s="1">
         <v>0</v>
@@ -17335,7 +17379,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="1">
-        <v>0</v>
+        <v>2.1</v>
       </c>
       <c r="M6" s="1">
         <v>0</v>
@@ -17347,10 +17391,10 @@
         <v>0</v>
       </c>
       <c r="P6" s="1">
-        <v>0</v>
+        <v>9.6</v>
       </c>
       <c r="Q6" s="1">
-        <v>0</v>
+        <v>19.8</v>
       </c>
       <c r="R6" s="1">
         <v>0</v>
@@ -17374,7 +17418,8 @@
         <v>0</v>
       </c>
       <c r="Y6" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>36.599999999999994</v>
       </c>
       <c r="Z6">
         <v>2022</v>
@@ -17403,19 +17448,19 @@
         <v>0</v>
       </c>
       <c r="F7" s="1">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="G7" s="1">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="H7" s="1">
         <v>0</v>
       </c>
       <c r="I7" s="1">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J7" s="1">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K7" s="1">
         <v>0</v>
@@ -17433,10 +17478,10 @@
         <v>0</v>
       </c>
       <c r="P7" s="1">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="Q7" s="1">
-        <v>0</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="R7" s="1">
         <v>0</v>
@@ -17460,7 +17505,8 @@
         <v>0</v>
       </c>
       <c r="Y7" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>20.8</v>
       </c>
       <c r="Z7">
         <v>2022</v>
@@ -17489,28 +17535,28 @@
         <v>0</v>
       </c>
       <c r="F8" s="1">
-        <v>0</v>
+        <v>100.5</v>
       </c>
       <c r="G8" s="1">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="H8" s="1">
-        <v>0</v>
+        <v>25.5</v>
       </c>
       <c r="I8" s="1">
-        <v>0</v>
+        <v>21.3</v>
       </c>
       <c r="J8" s="1">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="K8" s="1">
         <v>0</v>
       </c>
       <c r="L8" s="1">
-        <v>0</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="M8" s="1">
-        <v>0</v>
+        <v>30.7</v>
       </c>
       <c r="N8" s="1">
         <v>0</v>
@@ -17519,13 +17565,13 @@
         <v>0</v>
       </c>
       <c r="P8" s="1">
-        <v>0</v>
+        <v>1349.8</v>
       </c>
       <c r="Q8" s="1">
-        <v>0</v>
+        <v>2790.1</v>
       </c>
       <c r="R8" s="1">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="S8" s="1">
         <v>0</v>
@@ -17546,7 +17592,8 @@
         <v>0</v>
       </c>
       <c r="Y8" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>4346.3999999999996</v>
       </c>
       <c r="Z8">
         <v>2022</v>
@@ -17563,40 +17610,40 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>0</v>
+        <v>21.8</v>
       </c>
       <c r="C9" s="1">
-        <v>0</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="D9" s="1">
-        <v>0</v>
+        <v>13.100000000000001</v>
       </c>
       <c r="E9" s="1">
         <v>0</v>
       </c>
       <c r="F9" s="1">
-        <v>0</v>
+        <v>455.90000000000003</v>
       </c>
       <c r="G9" s="1">
-        <v>0</v>
+        <v>9.1</v>
       </c>
       <c r="H9" s="1">
-        <v>0</v>
+        <v>446.8</v>
       </c>
       <c r="I9" s="1">
-        <v>0</v>
+        <v>72.900000000000006</v>
       </c>
       <c r="J9" s="1">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="K9" s="1">
         <v>0</v>
       </c>
       <c r="L9" s="1">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="M9" s="1">
-        <v>0</v>
+        <v>20.3</v>
       </c>
       <c r="N9" s="1">
         <v>0</v>
@@ -17605,13 +17652,13 @@
         <v>0</v>
       </c>
       <c r="P9" s="1">
-        <v>0</v>
+        <v>2132.9</v>
       </c>
       <c r="Q9" s="1">
-        <v>0</v>
+        <v>4006.5</v>
       </c>
       <c r="R9" s="1">
-        <v>0</v>
+        <v>112.1</v>
       </c>
       <c r="S9" s="1">
         <v>0</v>
@@ -17632,7 +17679,8 @@
         <v>0</v>
       </c>
       <c r="Y9" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>6822.4000000000005</v>
       </c>
       <c r="Z9">
         <v>2022</v>
@@ -17649,37 +17697,37 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>0</v>
+        <v>1665.2</v>
       </c>
       <c r="C10" s="1">
-        <v>0</v>
+        <v>682.40000000000009</v>
       </c>
       <c r="D10" s="1">
-        <v>0</v>
+        <v>982.80000000000007</v>
       </c>
       <c r="E10" s="1">
-        <v>0</v>
+        <v>3.8</v>
       </c>
       <c r="F10" s="1">
-        <v>0</v>
+        <v>353</v>
       </c>
       <c r="G10" s="1">
-        <v>0</v>
+        <v>237.60000000000002</v>
       </c>
       <c r="H10" s="1">
-        <v>0</v>
+        <v>115.4</v>
       </c>
       <c r="I10" s="1">
-        <v>0</v>
+        <v>664.8</v>
       </c>
       <c r="J10" s="1">
-        <v>0</v>
+        <v>246.7</v>
       </c>
       <c r="K10" s="1">
-        <v>0</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="L10" s="1">
-        <v>0</v>
+        <v>409.5</v>
       </c>
       <c r="M10" s="1">
         <v>0</v>
@@ -17688,16 +17736,16 @@
         <v>0</v>
       </c>
       <c r="O10" s="1">
-        <v>0</v>
+        <v>37.800000000000004</v>
       </c>
       <c r="P10" s="1">
-        <v>0</v>
+        <v>10977.900000000001</v>
       </c>
       <c r="Q10" s="1">
-        <v>0</v>
+        <v>14491.599999999999</v>
       </c>
       <c r="R10" s="1">
-        <v>0</v>
+        <v>311.7</v>
       </c>
       <c r="S10" s="1">
         <v>0</v>
@@ -17712,13 +17760,14 @@
         <v>0</v>
       </c>
       <c r="W10" s="1">
-        <v>0</v>
+        <v>39.9</v>
       </c>
       <c r="X10" s="1">
         <v>0</v>
       </c>
       <c r="Y10" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>28545.7</v>
       </c>
       <c r="Z10">
         <v>2022</v>
@@ -17735,28 +17784,28 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>0</v>
+        <v>123.6</v>
       </c>
       <c r="C11" s="1">
-        <v>0</v>
+        <v>50.7</v>
       </c>
       <c r="D11" s="1">
-        <v>0</v>
+        <v>72.899999999999991</v>
       </c>
       <c r="E11" s="1">
         <v>0</v>
       </c>
       <c r="F11" s="1">
-        <v>0</v>
+        <v>185.29999999999998</v>
       </c>
       <c r="G11" s="1">
-        <v>0</v>
+        <v>169.2</v>
       </c>
       <c r="H11" s="1">
-        <v>0</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="I11" s="1">
-        <v>0</v>
+        <v>29.1</v>
       </c>
       <c r="J11" s="1">
         <v>0</v>
@@ -17765,7 +17814,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="1">
-        <v>0</v>
+        <v>29.1</v>
       </c>
       <c r="M11" s="1">
         <v>0</v>
@@ -17777,13 +17826,13 @@
         <v>0</v>
       </c>
       <c r="P11" s="1">
-        <v>0</v>
+        <v>3069.8</v>
       </c>
       <c r="Q11" s="1">
-        <v>0</v>
+        <v>3759.7</v>
       </c>
       <c r="R11" s="1">
-        <v>0</v>
+        <v>23.6</v>
       </c>
       <c r="S11" s="1">
         <v>0</v>
@@ -17804,7 +17853,8 @@
         <v>0</v>
       </c>
       <c r="Y11" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>7191.1</v>
       </c>
       <c r="Z11">
         <v>2022</v>
@@ -17821,28 +17871,28 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>0</v>
+        <v>70.7</v>
       </c>
       <c r="C12" s="1">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="D12" s="1">
-        <v>0</v>
+        <v>41.7</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
       </c>
       <c r="F12" s="1">
-        <v>0</v>
+        <v>85.199999999999989</v>
       </c>
       <c r="G12" s="1">
-        <v>0</v>
+        <v>63.8</v>
       </c>
       <c r="H12" s="1">
-        <v>0</v>
+        <v>21.4</v>
       </c>
       <c r="I12" s="1">
-        <v>0</v>
+        <v>67.099999999999994</v>
       </c>
       <c r="J12" s="1">
         <v>0</v>
@@ -17851,7 +17901,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="1">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="M12" s="1">
         <v>0</v>
@@ -17863,13 +17913,13 @@
         <v>0</v>
       </c>
       <c r="P12" s="1">
-        <v>0</v>
+        <v>2787.4</v>
       </c>
       <c r="Q12" s="1">
-        <v>0</v>
+        <v>3234.1</v>
       </c>
       <c r="R12" s="1">
-        <v>0</v>
+        <v>46.4</v>
       </c>
       <c r="S12" s="1">
         <v>0</v>
@@ -17890,7 +17940,8 @@
         <v>0</v>
       </c>
       <c r="Y12" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>6290.9</v>
       </c>
       <c r="Z12">
         <v>2022</v>
@@ -17907,37 +17958,37 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="C13" s="1">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D13" s="1">
-        <v>0</v>
+        <v>2.1</v>
       </c>
       <c r="E13" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F13" s="1">
-        <v>0</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="G13" s="1">
-        <v>0</v>
+        <v>3.3</v>
       </c>
       <c r="H13" s="1">
-        <v>0</v>
+        <v>14.3</v>
       </c>
       <c r="I13" s="1">
-        <v>0</v>
+        <v>114.8</v>
       </c>
       <c r="J13" s="1">
-        <v>0</v>
+        <v>3.1</v>
       </c>
       <c r="K13" s="1">
         <v>0</v>
       </c>
       <c r="L13" s="1">
-        <v>0</v>
+        <v>111.7</v>
       </c>
       <c r="M13" s="1">
         <v>0</v>
@@ -17946,10 +17997,10 @@
         <v>0</v>
       </c>
       <c r="O13" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="P13" s="1">
-        <v>0</v>
+        <v>540.4</v>
       </c>
       <c r="Q13" s="1">
         <v>0</v>
@@ -17976,7 +18027,8 @@
         <v>0</v>
       </c>
       <c r="Y13" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>676.59999999999991</v>
       </c>
       <c r="Z13">
         <v>2022</v>
@@ -17993,28 +18045,28 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="C14" s="1">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="D14" s="1">
-        <v>0</v>
+        <v>0.79999999999999993</v>
       </c>
       <c r="E14" s="1">
         <v>0</v>
       </c>
       <c r="F14" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G14" s="1">
         <v>0</v>
       </c>
       <c r="H14" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I14" s="1">
-        <v>0</v>
+        <v>19.7</v>
       </c>
       <c r="J14" s="1">
         <v>0</v>
@@ -18023,7 +18075,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="1">
-        <v>0</v>
+        <v>19.7</v>
       </c>
       <c r="M14" s="1">
         <v>0</v>
@@ -18035,13 +18087,13 @@
         <v>0</v>
       </c>
       <c r="P14" s="1">
-        <v>0</v>
+        <v>29.1</v>
       </c>
       <c r="Q14" s="1">
         <v>0</v>
       </c>
       <c r="R14" s="1">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="S14" s="1">
         <v>0</v>
@@ -18062,7 +18114,8 @@
         <v>0</v>
       </c>
       <c r="Y14" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>53.8</v>
       </c>
       <c r="Z14">
         <v>2022</v>
@@ -18079,37 +18132,37 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="C15" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D15" s="1">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E15" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F15" s="1">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="G15" s="1">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="H15" s="1">
         <v>0</v>
       </c>
       <c r="I15" s="1">
-        <v>0</v>
+        <v>37.9</v>
       </c>
       <c r="J15" s="1">
-        <v>0</v>
+        <v>12.3</v>
       </c>
       <c r="K15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15" s="1">
-        <v>0</v>
+        <v>24.7</v>
       </c>
       <c r="M15" s="1">
         <v>0</v>
@@ -18121,7 +18174,7 @@
         <v>0</v>
       </c>
       <c r="P15" s="1">
-        <v>0</v>
+        <v>72.2</v>
       </c>
       <c r="Q15" s="1">
         <v>0</v>
@@ -18148,7 +18201,8 @@
         <v>0</v>
       </c>
       <c r="Y15" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>113.2</v>
       </c>
       <c r="Z15">
         <v>2022</v>
@@ -18177,25 +18231,25 @@
         <v>0</v>
       </c>
       <c r="F16" s="1">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="G16" s="1">
         <v>0</v>
       </c>
       <c r="H16" s="1">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I16" s="1">
-        <v>0</v>
+        <v>95.7</v>
       </c>
       <c r="J16" s="1">
-        <v>0</v>
+        <v>48.2</v>
       </c>
       <c r="K16" s="1">
-        <v>0</v>
+        <v>7.8</v>
       </c>
       <c r="L16" s="1">
-        <v>0</v>
+        <v>39.9</v>
       </c>
       <c r="M16" s="1">
         <v>0</v>
@@ -18207,7 +18261,7 @@
         <v>0</v>
       </c>
       <c r="P16" s="1">
-        <v>0</v>
+        <v>160.5</v>
       </c>
       <c r="Q16" s="1">
         <v>0</v>
@@ -18234,7 +18288,8 @@
         <v>0</v>
       </c>
       <c r="Y16" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>257.7</v>
       </c>
       <c r="Z16">
         <v>2022</v>
@@ -18251,37 +18306,37 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="C17" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D17" s="1">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E17" s="1">
         <v>0</v>
       </c>
       <c r="F17" s="1">
-        <v>0</v>
+        <v>12.2</v>
       </c>
       <c r="G17" s="1">
         <v>0</v>
       </c>
       <c r="H17" s="1">
-        <v>0</v>
+        <v>12.2</v>
       </c>
       <c r="I17" s="1">
-        <v>0</v>
+        <v>10.4</v>
       </c>
       <c r="J17" s="1">
-        <v>0</v>
+        <v>7.9</v>
       </c>
       <c r="K17" s="1">
         <v>0</v>
       </c>
       <c r="L17" s="1">
-        <v>0</v>
+        <v>2.6</v>
       </c>
       <c r="M17" s="1">
         <v>0</v>
@@ -18293,10 +18348,10 @@
         <v>0</v>
       </c>
       <c r="P17" s="1">
-        <v>0</v>
+        <v>83.9</v>
       </c>
       <c r="Q17" s="1">
-        <v>0</v>
+        <v>9.1</v>
       </c>
       <c r="R17" s="1">
         <v>0</v>
@@ -18320,7 +18375,8 @@
         <v>0</v>
       </c>
       <c r="Y17" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>116.9</v>
       </c>
       <c r="Z17">
         <v>2022</v>
@@ -18349,19 +18405,19 @@
         <v>0</v>
       </c>
       <c r="F18" s="1">
-        <v>0</v>
+        <v>46.9</v>
       </c>
       <c r="G18" s="1">
         <v>0</v>
       </c>
       <c r="H18" s="1">
-        <v>0</v>
+        <v>46.9</v>
       </c>
       <c r="I18" s="1">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="J18" s="1">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="K18" s="1">
         <v>0</v>
@@ -18379,7 +18435,7 @@
         <v>0</v>
       </c>
       <c r="P18" s="1">
-        <v>0</v>
+        <v>949.1</v>
       </c>
       <c r="Q18" s="1">
         <v>0</v>
@@ -18406,7 +18462,8 @@
         <v>0</v>
       </c>
       <c r="Y18" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>998.7</v>
       </c>
       <c r="Z18">
         <v>2022</v>
@@ -18423,16 +18480,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>0</v>
+        <v>1463.9</v>
       </c>
       <c r="C19" s="1">
-        <v>0</v>
+        <v>600.20000000000005</v>
       </c>
       <c r="D19" s="1">
-        <v>0</v>
+        <v>863.7</v>
       </c>
       <c r="E19" s="1">
-        <v>0</v>
+        <v>2.8</v>
       </c>
       <c r="F19" s="1">
         <v>0</v>
@@ -18444,16 +18501,16 @@
         <v>0</v>
       </c>
       <c r="I19" s="1">
-        <v>0</v>
+        <v>287.39999999999998</v>
       </c>
       <c r="J19" s="1">
-        <v>0</v>
+        <v>172.5</v>
       </c>
       <c r="K19" s="1">
         <v>0</v>
       </c>
       <c r="L19" s="1">
-        <v>0</v>
+        <v>114.8</v>
       </c>
       <c r="M19" s="1">
         <v>0</v>
@@ -18462,16 +18519,16 @@
         <v>0</v>
       </c>
       <c r="O19" s="1">
-        <v>0</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="P19" s="1">
-        <v>0</v>
+        <v>3285.5</v>
       </c>
       <c r="Q19" s="1">
-        <v>0</v>
+        <v>7488.7</v>
       </c>
       <c r="R19" s="1">
-        <v>0</v>
+        <v>240.9</v>
       </c>
       <c r="S19" s="1">
         <v>0</v>
@@ -18486,13 +18543,14 @@
         <v>0</v>
       </c>
       <c r="W19" s="1">
-        <v>0</v>
+        <v>39.9</v>
       </c>
       <c r="X19" s="1">
         <v>0</v>
       </c>
       <c r="Y19" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>12846.8</v>
       </c>
       <c r="Z19">
         <v>2022</v>
@@ -18509,58 +18567,58 @@
         <v>57</v>
       </c>
       <c r="B20" s="1">
-        <v>0</v>
+        <v>5347.3</v>
       </c>
       <c r="C20" s="1">
-        <v>0</v>
+        <v>2206.8999999999996</v>
       </c>
       <c r="D20" s="1">
-        <v>0</v>
+        <v>3140.3999999999996</v>
       </c>
       <c r="E20" s="1">
-        <v>0</v>
+        <v>22.2</v>
       </c>
       <c r="F20" s="1">
-        <v>0</v>
+        <v>435.2</v>
       </c>
       <c r="G20" s="1">
-        <v>0</v>
+        <v>286.79999999999995</v>
       </c>
       <c r="H20" s="1">
-        <v>0</v>
+        <v>148.4</v>
       </c>
       <c r="I20" s="1">
-        <v>0</v>
+        <v>578.20000000000005</v>
       </c>
       <c r="J20" s="1">
-        <v>0</v>
+        <v>477.1</v>
       </c>
       <c r="K20" s="1">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="L20" s="1">
-        <v>0</v>
+        <v>98.3</v>
       </c>
       <c r="M20" s="1">
-        <v>0</v>
+        <v>59.9</v>
       </c>
       <c r="N20" s="1">
-        <v>0</v>
+        <v>52.2</v>
       </c>
       <c r="O20" s="1">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="P20" s="1">
-        <v>0</v>
+        <v>69269.099999999991</v>
       </c>
       <c r="Q20" s="1">
-        <v>0</v>
+        <v>72624.3</v>
       </c>
       <c r="R20" s="1">
-        <v>0</v>
+        <v>1725.5</v>
       </c>
       <c r="S20" s="1">
-        <v>0</v>
+        <v>74.3</v>
       </c>
       <c r="T20" s="1">
         <v>0</v>
@@ -18572,13 +18630,14 @@
         <v>0</v>
       </c>
       <c r="W20" s="1">
-        <v>0</v>
+        <v>194.29999999999998</v>
       </c>
       <c r="X20" s="1">
         <v>0</v>
       </c>
       <c r="Y20" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>150383.19999999995</v>
       </c>
       <c r="Z20">
         <v>2022</v>
@@ -18595,55 +18654,55 @@
         <v>19</v>
       </c>
       <c r="B21" s="1">
-        <v>0</v>
+        <v>5082.8999999999996</v>
       </c>
       <c r="C21" s="1">
-        <v>0</v>
+        <v>2099.1999999999998</v>
       </c>
       <c r="D21" s="1">
-        <v>0</v>
+        <v>2983.7</v>
       </c>
       <c r="E21" s="1">
         <v>0</v>
       </c>
       <c r="F21" s="1">
-        <v>0</v>
+        <v>300.59999999999997</v>
       </c>
       <c r="G21" s="1">
-        <v>0</v>
+        <v>278.39999999999998</v>
       </c>
       <c r="H21" s="1">
-        <v>0</v>
+        <v>22.2</v>
       </c>
       <c r="I21" s="1">
-        <v>0</v>
+        <v>261.8</v>
       </c>
       <c r="J21" s="1">
-        <v>0</v>
+        <v>180.1</v>
       </c>
       <c r="K21" s="1">
         <v>0</v>
       </c>
       <c r="L21" s="1">
-        <v>0</v>
+        <v>81.7</v>
       </c>
       <c r="M21" s="1">
-        <v>0</v>
+        <v>58.4</v>
       </c>
       <c r="N21" s="1">
-        <v>0</v>
+        <v>13.3</v>
       </c>
       <c r="O21" s="1">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="P21" s="1">
-        <v>0</v>
+        <v>44614.7</v>
       </c>
       <c r="Q21" s="1">
-        <v>0</v>
+        <v>41538.300000000003</v>
       </c>
       <c r="R21" s="1">
-        <v>0</v>
+        <v>174.9</v>
       </c>
       <c r="S21" s="1">
         <v>0</v>
@@ -18664,7 +18723,8 @@
         <v>0</v>
       </c>
       <c r="Y21" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>92045.599999999991</v>
       </c>
       <c r="Z21">
         <v>2022</v>
@@ -18681,31 +18741,31 @@
         <v>20</v>
       </c>
       <c r="B22" s="1">
-        <v>0</v>
+        <v>141.6</v>
       </c>
       <c r="C22" s="1">
-        <v>0</v>
+        <v>58.6</v>
       </c>
       <c r="D22" s="1">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="E22" s="1">
-        <v>0</v>
+        <v>22.2</v>
       </c>
       <c r="F22" s="1">
-        <v>0</v>
+        <v>49.3</v>
       </c>
       <c r="G22" s="1">
         <v>0</v>
       </c>
       <c r="H22" s="1">
-        <v>0</v>
+        <v>49.3</v>
       </c>
       <c r="I22" s="1">
-        <v>0</v>
+        <v>13.1</v>
       </c>
       <c r="J22" s="1">
-        <v>0</v>
+        <v>13.1</v>
       </c>
       <c r="K22" s="1">
         <v>0</v>
@@ -18723,16 +18783,16 @@
         <v>0</v>
       </c>
       <c r="P22" s="1">
-        <v>0</v>
+        <v>11159.3</v>
       </c>
       <c r="Q22" s="1">
-        <v>0</v>
+        <v>13347.1</v>
       </c>
       <c r="R22" s="1">
-        <v>0</v>
+        <v>340.3</v>
       </c>
       <c r="S22" s="1">
-        <v>0</v>
+        <v>74.3</v>
       </c>
       <c r="T22" s="1">
         <v>0</v>
@@ -18744,13 +18804,14 @@
         <v>0</v>
       </c>
       <c r="W22" s="1">
-        <v>0</v>
+        <v>48.6</v>
       </c>
       <c r="X22" s="1">
         <v>0</v>
       </c>
       <c r="Y22" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>25195.799999999996</v>
       </c>
       <c r="Z22">
         <v>2022</v>
@@ -18767,55 +18828,55 @@
         <v>21</v>
       </c>
       <c r="B23" s="1">
-        <v>0</v>
+        <v>122.8</v>
       </c>
       <c r="C23" s="1">
-        <v>0</v>
+        <v>49.1</v>
       </c>
       <c r="D23" s="1">
-        <v>0</v>
+        <v>73.699999999999989</v>
       </c>
       <c r="E23" s="1">
         <v>0</v>
       </c>
       <c r="F23" s="1">
-        <v>0</v>
+        <v>85.300000000000011</v>
       </c>
       <c r="G23" s="1">
-        <v>0</v>
+        <v>8.4</v>
       </c>
       <c r="H23" s="1">
-        <v>0</v>
+        <v>76.900000000000006</v>
       </c>
       <c r="I23" s="1">
-        <v>0</v>
+        <v>264.5</v>
       </c>
       <c r="J23" s="1">
-        <v>0</v>
+        <v>247.9</v>
       </c>
       <c r="K23" s="1">
         <v>0</v>
       </c>
       <c r="L23" s="1">
-        <v>0</v>
+        <v>16.5</v>
       </c>
       <c r="M23" s="1">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="N23" s="1">
-        <v>0</v>
+        <v>37.4</v>
       </c>
       <c r="O23" s="1">
         <v>0</v>
       </c>
       <c r="P23" s="1">
-        <v>0</v>
+        <v>12990.7</v>
       </c>
       <c r="Q23" s="1">
-        <v>0</v>
+        <v>17420.400000000001</v>
       </c>
       <c r="R23" s="1">
-        <v>0</v>
+        <v>1174.5</v>
       </c>
       <c r="S23" s="1">
         <v>0</v>
@@ -18830,13 +18891,14 @@
         <v>0</v>
       </c>
       <c r="W23" s="1">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="X23" s="1">
         <v>0</v>
       </c>
       <c r="Y23" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>32232.100000000002</v>
       </c>
       <c r="Z23">
         <v>2022</v>
@@ -18874,34 +18936,34 @@
         <v>0</v>
       </c>
       <c r="I24" s="1">
-        <v>0</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="J24" s="1">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="K24" s="1">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="L24" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="M24" s="1">
         <v>0</v>
       </c>
       <c r="N24" s="1">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="O24" s="1">
         <v>0</v>
       </c>
       <c r="P24" s="1">
-        <v>0</v>
+        <v>504.4</v>
       </c>
       <c r="Q24" s="1">
-        <v>0</v>
+        <v>318.5</v>
       </c>
       <c r="R24" s="1">
-        <v>0</v>
+        <v>35.799999999999997</v>
       </c>
       <c r="S24" s="1">
         <v>0</v>
@@ -18916,13 +18978,14 @@
         <v>0</v>
       </c>
       <c r="W24" s="1">
-        <v>0</v>
+        <v>10.7</v>
       </c>
       <c r="X24" s="1">
         <v>0</v>
       </c>
       <c r="Y24" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>909.69999999999993</v>
       </c>
       <c r="Z24">
         <v>2022</v>
@@ -18939,55 +19002,55 @@
         <v>23</v>
       </c>
       <c r="B25" s="1">
-        <v>0</v>
+        <v>162.60000000000002</v>
       </c>
       <c r="C25" s="1">
-        <v>0</v>
+        <v>67.900000000000006</v>
       </c>
       <c r="D25" s="1">
-        <v>0</v>
+        <v>94.7</v>
       </c>
       <c r="E25" s="1">
-        <v>0</v>
+        <v>767.3</v>
       </c>
       <c r="F25" s="1">
-        <v>0</v>
+        <v>52.099999999999994</v>
       </c>
       <c r="G25" s="1">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="H25" s="1">
-        <v>0</v>
+        <v>44.599999999999994</v>
       </c>
       <c r="I25" s="1">
-        <v>0</v>
+        <v>648.70000000000005</v>
       </c>
       <c r="J25" s="1">
-        <v>0</v>
+        <v>628.69999999999993</v>
       </c>
       <c r="K25" s="1">
-        <v>0</v>
+        <v>12.799999999999999</v>
       </c>
       <c r="L25" s="1">
-        <v>0</v>
+        <v>7.3999999999999995</v>
       </c>
       <c r="M25" s="1">
         <v>0</v>
       </c>
       <c r="N25" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O25" s="1">
         <v>0</v>
       </c>
       <c r="P25" s="1">
-        <v>0</v>
+        <v>13161.100000000002</v>
       </c>
       <c r="Q25" s="1">
-        <v>0</v>
+        <v>12363.7</v>
       </c>
       <c r="R25" s="1">
-        <v>0</v>
+        <v>712</v>
       </c>
       <c r="S25" s="1">
         <v>0</v>
@@ -19002,13 +19065,14 @@
         <v>0</v>
       </c>
       <c r="W25" s="1">
-        <v>0</v>
+        <v>606.09999999999991</v>
       </c>
       <c r="X25" s="1">
-        <v>0</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="Y25" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>28481.500000000004</v>
       </c>
       <c r="Z25">
         <v>2022</v>
@@ -19025,55 +19089,55 @@
         <v>24</v>
       </c>
       <c r="B26" s="1">
-        <v>0</v>
+        <v>116.9</v>
       </c>
       <c r="C26" s="1">
-        <v>0</v>
+        <v>47.7</v>
       </c>
       <c r="D26" s="1">
-        <v>0</v>
+        <v>69.2</v>
       </c>
       <c r="E26" s="1">
-        <v>0</v>
+        <v>21.5</v>
       </c>
       <c r="F26" s="1">
-        <v>0</v>
+        <v>9.1</v>
       </c>
       <c r="G26" s="1">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="H26" s="1">
-        <v>0</v>
+        <v>7.3</v>
       </c>
       <c r="I26" s="1">
-        <v>0</v>
+        <v>470.3</v>
       </c>
       <c r="J26" s="1">
-        <v>0</v>
+        <v>451.4</v>
       </c>
       <c r="K26" s="1">
-        <v>0</v>
+        <v>11.7</v>
       </c>
       <c r="L26" s="1">
-        <v>0</v>
+        <v>7.3999999999999995</v>
       </c>
       <c r="M26" s="1">
         <v>0</v>
       </c>
       <c r="N26" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O26" s="1">
         <v>0</v>
       </c>
       <c r="P26" s="1">
-        <v>0</v>
+        <v>8917.6</v>
       </c>
       <c r="Q26" s="1">
-        <v>0</v>
+        <v>7868</v>
       </c>
       <c r="R26" s="1">
-        <v>0</v>
+        <v>669.7</v>
       </c>
       <c r="S26" s="1">
         <v>0</v>
@@ -19088,13 +19152,14 @@
         <v>0</v>
       </c>
       <c r="W26" s="1">
-        <v>0</v>
+        <v>298.7</v>
       </c>
       <c r="X26" s="1">
         <v>0</v>
       </c>
       <c r="Y26" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>18374.800000000003</v>
       </c>
       <c r="Z26">
         <v>2022</v>
@@ -19134,19 +19199,19 @@
         <v>0</v>
       </c>
       <c r="F27" s="1">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G27" s="1">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="H27" s="1">
         <v>0</v>
       </c>
       <c r="I27" s="1">
-        <v>0</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="J27" s="1">
-        <v>0</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="K27" s="1">
         <v>0</v>
@@ -19164,7 +19229,7 @@
         <v>0</v>
       </c>
       <c r="P27" s="1">
-        <v>0</v>
+        <v>40.200000000000003</v>
       </c>
       <c r="Q27" s="1">
         <v>0</v>
@@ -19191,7 +19256,8 @@
         <v>0</v>
       </c>
       <c r="Y27" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>50.300000000000004</v>
       </c>
       <c r="Z27">
         <v>2022</v>
@@ -19220,22 +19286,22 @@
         <v>0</v>
       </c>
       <c r="F28" s="1">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="G28" s="1">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="H28" s="1">
         <v>0</v>
       </c>
       <c r="I28" s="1">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J28" s="1">
         <v>0</v>
       </c>
       <c r="K28" s="1">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="L28" s="1">
         <v>0</v>
@@ -19250,7 +19316,7 @@
         <v>0</v>
       </c>
       <c r="P28" s="1">
-        <v>0</v>
+        <v>7.1</v>
       </c>
       <c r="Q28" s="1">
         <v>0</v>
@@ -19277,7 +19343,8 @@
         <v>0</v>
       </c>
       <c r="Y28" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>9.1</v>
       </c>
       <c r="Z28">
         <v>2022</v>
@@ -19294,31 +19361,31 @@
         <v>27</v>
       </c>
       <c r="B29" s="1">
-        <v>0</v>
+        <v>45.7</v>
       </c>
       <c r="C29" s="1">
-        <v>0</v>
+        <v>20.2</v>
       </c>
       <c r="D29" s="1">
-        <v>0</v>
+        <v>25.500000000000004</v>
       </c>
       <c r="E29" s="1">
-        <v>0</v>
+        <v>745.8</v>
       </c>
       <c r="F29" s="1">
-        <v>0</v>
+        <v>41.699999999999996</v>
       </c>
       <c r="G29" s="1">
-        <v>0</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="H29" s="1">
-        <v>0</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="I29" s="1">
-        <v>0</v>
+        <v>167.6</v>
       </c>
       <c r="J29" s="1">
-        <v>0</v>
+        <v>167.6</v>
       </c>
       <c r="K29" s="1">
         <v>0</v>
@@ -19336,13 +19403,13 @@
         <v>0</v>
       </c>
       <c r="P29" s="1">
-        <v>0</v>
+        <v>4196.2</v>
       </c>
       <c r="Q29" s="1">
-        <v>0</v>
+        <v>4495.7</v>
       </c>
       <c r="R29" s="1">
-        <v>0</v>
+        <v>42.3</v>
       </c>
       <c r="S29" s="1">
         <v>0</v>
@@ -19357,13 +19424,14 @@
         <v>0</v>
       </c>
       <c r="W29" s="1">
-        <v>0</v>
+        <v>307.39999999999998</v>
       </c>
       <c r="X29" s="1">
-        <v>0</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="Y29" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>10047.299999999999</v>
       </c>
       <c r="Z29">
         <v>2022</v>
@@ -19380,34 +19448,34 @@
         <v>28</v>
       </c>
       <c r="B30" s="1">
-        <v>0</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="C30" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D30" s="1">
-        <v>0</v>
+        <v>2.9000000000000004</v>
       </c>
       <c r="E30" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F30" s="1">
-        <v>0</v>
+        <v>9056</v>
       </c>
       <c r="G30" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H30" s="1">
-        <v>0</v>
+        <v>9053</v>
       </c>
       <c r="I30" s="1">
-        <v>0</v>
+        <v>901.3</v>
       </c>
       <c r="J30" s="1">
-        <v>0</v>
+        <v>361</v>
       </c>
       <c r="K30" s="1">
-        <v>0</v>
+        <v>540.29999999999995</v>
       </c>
       <c r="L30" s="1">
         <v>0</v>
@@ -19416,40 +19484,41 @@
         <v>0</v>
       </c>
       <c r="N30" s="1">
-        <v>0</v>
+        <v>5.2</v>
       </c>
       <c r="O30" s="1">
         <v>0</v>
       </c>
       <c r="P30" s="1">
-        <v>0</v>
+        <v>27770.1</v>
       </c>
       <c r="Q30" s="1">
-        <v>0</v>
+        <v>45130.399999999994</v>
       </c>
       <c r="R30" s="1">
-        <v>0</v>
+        <v>52.9</v>
       </c>
       <c r="S30" s="1">
-        <v>0</v>
+        <v>1101.3</v>
       </c>
       <c r="T30" s="1">
-        <v>0</v>
+        <v>83.3</v>
       </c>
       <c r="U30" s="1">
-        <v>0</v>
+        <v>12.399999999999999</v>
       </c>
       <c r="V30" s="1">
-        <v>0</v>
+        <v>496.79999999999995</v>
       </c>
       <c r="W30" s="1">
-        <v>0</v>
+        <v>8660.6</v>
       </c>
       <c r="X30" s="1">
-        <v>0</v>
+        <v>52.900000000000006</v>
       </c>
       <c r="Y30" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>93337.099999999991</v>
       </c>
       <c r="Z30">
         <v>2022</v>
@@ -19466,34 +19535,34 @@
         <v>29</v>
       </c>
       <c r="B31" s="1">
-        <v>0</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="C31" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D31" s="1">
-        <v>0</v>
+        <v>2.9000000000000004</v>
       </c>
       <c r="E31" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F31" s="1">
-        <v>0</v>
+        <v>153.4</v>
       </c>
       <c r="G31" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H31" s="1">
-        <v>0</v>
+        <v>150.4</v>
       </c>
       <c r="I31" s="1">
-        <v>0</v>
+        <v>721.3</v>
       </c>
       <c r="J31" s="1">
-        <v>0</v>
+        <v>313.8</v>
       </c>
       <c r="K31" s="1">
-        <v>0</v>
+        <v>407.5</v>
       </c>
       <c r="L31" s="1">
         <v>0</v>
@@ -19508,34 +19577,35 @@
         <v>0</v>
       </c>
       <c r="P31" s="1">
-        <v>0</v>
+        <v>19254.3</v>
       </c>
       <c r="Q31" s="1">
-        <v>0</v>
+        <v>20804.3</v>
       </c>
       <c r="R31" s="1">
-        <v>0</v>
+        <v>52.9</v>
       </c>
       <c r="S31" s="1">
-        <v>0</v>
+        <v>241.2</v>
       </c>
       <c r="T31" s="1">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="U31" s="1">
-        <v>0</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="V31" s="1">
-        <v>0</v>
+        <v>372.4</v>
       </c>
       <c r="W31" s="1">
-        <v>0</v>
+        <v>3624.8</v>
       </c>
       <c r="X31" s="1">
-        <v>0</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="Y31" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>45277.599999999991</v>
       </c>
       <c r="Z31">
         <v>2022</v>
@@ -19564,22 +19634,22 @@
         <v>0</v>
       </c>
       <c r="F32" s="1">
-        <v>0</v>
+        <v>1208.2</v>
       </c>
       <c r="G32" s="1">
         <v>0</v>
       </c>
       <c r="H32" s="1">
-        <v>0</v>
+        <v>1208.2</v>
       </c>
       <c r="I32" s="1">
-        <v>0</v>
+        <v>110.3</v>
       </c>
       <c r="J32" s="1">
-        <v>0</v>
+        <v>25.3</v>
       </c>
       <c r="K32" s="1">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="L32" s="1">
         <v>0</v>
@@ -19594,10 +19664,10 @@
         <v>0</v>
       </c>
       <c r="P32" s="1">
-        <v>0</v>
+        <v>2685.3</v>
       </c>
       <c r="Q32" s="1">
-        <v>0</v>
+        <v>2498</v>
       </c>
       <c r="R32" s="1">
         <v>0</v>
@@ -19612,16 +19682,17 @@
         <v>0</v>
       </c>
       <c r="V32" s="1">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="W32" s="1">
-        <v>0</v>
+        <v>475.7</v>
       </c>
       <c r="X32" s="1">
         <v>0</v>
       </c>
       <c r="Y32" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>6979.2</v>
       </c>
       <c r="Z32">
         <v>2022</v>
@@ -19647,25 +19718,25 @@
         <v>0</v>
       </c>
       <c r="E33" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F33" s="1">
-        <v>0</v>
+        <v>7694.4</v>
       </c>
       <c r="G33" s="1">
         <v>0</v>
       </c>
       <c r="H33" s="1">
-        <v>0</v>
+        <v>7694.4</v>
       </c>
       <c r="I33" s="1">
-        <v>0</v>
+        <v>69.7</v>
       </c>
       <c r="J33" s="1">
-        <v>0</v>
+        <v>21.9</v>
       </c>
       <c r="K33" s="1">
-        <v>0</v>
+        <v>47.8</v>
       </c>
       <c r="L33" s="1">
         <v>0</v>
@@ -19674,40 +19745,41 @@
         <v>0</v>
       </c>
       <c r="N33" s="1">
-        <v>0</v>
+        <v>5.2</v>
       </c>
       <c r="O33" s="1">
         <v>0</v>
       </c>
       <c r="P33" s="1">
-        <v>0</v>
+        <v>5830.5</v>
       </c>
       <c r="Q33" s="1">
-        <v>0</v>
+        <v>21828.1</v>
       </c>
       <c r="R33" s="1">
         <v>0</v>
       </c>
       <c r="S33" s="1">
-        <v>0</v>
+        <v>860.1</v>
       </c>
       <c r="T33" s="1">
-        <v>0</v>
+        <v>82.1</v>
       </c>
       <c r="U33" s="1">
-        <v>0</v>
+        <v>3.7</v>
       </c>
       <c r="V33" s="1">
-        <v>0</v>
+        <v>122.7</v>
       </c>
       <c r="W33" s="1">
-        <v>0</v>
+        <v>4560.1000000000004</v>
       </c>
       <c r="X33" s="1">
-        <v>0</v>
+        <v>18.7</v>
       </c>
       <c r="Y33" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>41080.299999999981</v>
       </c>
       <c r="Z33">
         <v>2022</v>
@@ -19724,55 +19796,55 @@
         <v>58</v>
       </c>
       <c r="B34" s="1">
-        <v>0</v>
+        <v>1718.6000000000001</v>
       </c>
       <c r="C34" s="1">
-        <v>0</v>
+        <v>703.10000000000014</v>
       </c>
       <c r="D34" s="1">
-        <v>0</v>
+        <v>1015.5000000000001</v>
       </c>
       <c r="E34" s="1">
-        <v>0</v>
+        <v>3.8</v>
       </c>
       <c r="F34" s="1">
-        <v>0</v>
+        <v>1096.2</v>
       </c>
       <c r="G34" s="1">
-        <v>0</v>
+        <v>417.4</v>
       </c>
       <c r="H34" s="1">
-        <v>0</v>
+        <v>678.8</v>
       </c>
       <c r="I34" s="1">
-        <v>0</v>
+        <v>771.69999999999993</v>
       </c>
       <c r="J34" s="1">
-        <v>0</v>
+        <v>254.6</v>
       </c>
       <c r="K34" s="1">
-        <v>0</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="L34" s="1">
-        <v>0</v>
+        <v>508.5</v>
       </c>
       <c r="M34" s="1">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="N34" s="1">
         <v>0</v>
       </c>
       <c r="O34" s="1">
-        <v>0</v>
+        <v>37.800000000000004</v>
       </c>
       <c r="P34" s="1">
-        <v>0</v>
+        <v>16197.000000000002</v>
       </c>
       <c r="Q34" s="1">
-        <v>0</v>
+        <v>23419.8</v>
       </c>
       <c r="R34" s="1">
-        <v>0</v>
+        <v>477.79999999999995</v>
       </c>
       <c r="S34" s="1">
         <v>0</v>
@@ -19787,13 +19859,14 @@
         <v>0</v>
       </c>
       <c r="W34" s="1">
-        <v>0</v>
+        <v>39.9</v>
       </c>
       <c r="X34" s="1">
         <v>0</v>
       </c>
       <c r="Y34" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>43813.600000000006</v>
       </c>
       <c r="Z34">
         <v>2022</v>
@@ -19810,76 +19883,77 @@
         <v>59</v>
       </c>
       <c r="B35" s="1">
-        <v>0</v>
+        <v>5514.8</v>
       </c>
       <c r="C35" s="1">
-        <v>0</v>
+        <v>2276.7999999999997</v>
       </c>
       <c r="D35" s="1">
-        <v>0</v>
+        <v>3237.9999999999995</v>
       </c>
       <c r="E35" s="1">
-        <v>0</v>
+        <v>798.5</v>
       </c>
       <c r="F35" s="1">
-        <v>0</v>
+        <v>9543.2999999999993</v>
       </c>
       <c r="G35" s="1">
-        <v>0</v>
+        <v>297.29999999999995</v>
       </c>
       <c r="H35" s="1">
-        <v>0</v>
+        <v>9246</v>
       </c>
       <c r="I35" s="1">
-        <v>0</v>
+        <v>2128.1999999999998</v>
       </c>
       <c r="J35" s="1">
-        <v>0</v>
+        <v>1466.8</v>
       </c>
       <c r="K35" s="1">
-        <v>0</v>
+        <v>555.79999999999995</v>
       </c>
       <c r="L35" s="1">
-        <v>0</v>
+        <v>105.7</v>
       </c>
       <c r="M35" s="1">
-        <v>0</v>
+        <v>59.9</v>
       </c>
       <c r="N35" s="1">
-        <v>0</v>
+        <v>60.400000000000006</v>
       </c>
       <c r="O35" s="1">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="P35" s="1">
-        <v>0</v>
+        <v>110200.29999999999</v>
       </c>
       <c r="Q35" s="1">
-        <v>0</v>
+        <v>130118.39999999999</v>
       </c>
       <c r="R35" s="1">
-        <v>0</v>
+        <v>2490.4</v>
       </c>
       <c r="S35" s="1">
-        <v>0</v>
+        <v>1175.5999999999999</v>
       </c>
       <c r="T35" s="1">
-        <v>0</v>
+        <v>83.3</v>
       </c>
       <c r="U35" s="1">
-        <v>0</v>
+        <v>12.399999999999999</v>
       </c>
       <c r="V35" s="1">
-        <v>0</v>
+        <v>496.79999999999995</v>
       </c>
       <c r="W35" s="1">
-        <v>0</v>
+        <v>9461</v>
       </c>
       <c r="X35" s="1">
-        <v>0</v>
+        <v>57.800000000000004</v>
       </c>
       <c r="Y35" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>272201.8</v>
       </c>
       <c r="Z35">
         <v>2022</v>
@@ -19896,76 +19970,77 @@
         <v>32</v>
       </c>
       <c r="B36" s="1">
-        <v>0</v>
+        <v>7233.4000000000005</v>
       </c>
       <c r="C36" s="1">
-        <v>0</v>
+        <v>2979.9</v>
       </c>
       <c r="D36" s="1">
-        <v>0</v>
+        <v>4253.4999999999991</v>
       </c>
       <c r="E36" s="1">
-        <v>0</v>
+        <v>802.3</v>
       </c>
       <c r="F36" s="1">
-        <v>0</v>
+        <v>10639.5</v>
       </c>
       <c r="G36" s="1">
-        <v>0</v>
+        <v>714.69999999999993</v>
       </c>
       <c r="H36" s="1">
-        <v>0</v>
+        <v>9924.7999999999993</v>
       </c>
       <c r="I36" s="1">
-        <v>0</v>
+        <v>2899.8999999999996</v>
       </c>
       <c r="J36" s="1">
-        <v>0</v>
+        <v>1721.3999999999999</v>
       </c>
       <c r="K36" s="1">
-        <v>0</v>
+        <v>564.59999999999991</v>
       </c>
       <c r="L36" s="1">
-        <v>0</v>
+        <v>614.20000000000005</v>
       </c>
       <c r="M36" s="1">
-        <v>0</v>
+        <v>110.9</v>
       </c>
       <c r="N36" s="1">
-        <v>0</v>
+        <v>60.400000000000006</v>
       </c>
       <c r="O36" s="1">
-        <v>0</v>
+        <v>38.500000000000007</v>
       </c>
       <c r="P36" s="1">
-        <v>0</v>
+        <v>126397.29999999999</v>
       </c>
       <c r="Q36" s="1">
-        <v>0</v>
+        <v>153538.19999999998</v>
       </c>
       <c r="R36" s="1">
-        <v>0</v>
+        <v>2968.2</v>
       </c>
       <c r="S36" s="1">
-        <v>0</v>
+        <v>1175.5999999999999</v>
       </c>
       <c r="T36" s="1">
-        <v>0</v>
+        <v>83.3</v>
       </c>
       <c r="U36" s="1">
-        <v>0</v>
+        <v>12.399999999999999</v>
       </c>
       <c r="V36" s="1">
-        <v>0</v>
+        <v>496.79999999999995</v>
       </c>
       <c r="W36" s="1">
-        <v>0</v>
+        <v>9500.9</v>
       </c>
       <c r="X36" s="1">
-        <v>0</v>
+        <v>57.800000000000004</v>
       </c>
       <c r="Y36" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>316015.39999999997</v>
       </c>
       <c r="Z36">
         <v>2022</v>

</xml_diff>

<commit_message>
feat: dados de Dezembro 2022 tratados
</commit_message>
<xml_diff>
--- a/Base de Dados/Dados Tratados/NOVEMBRO_2022.xlsx
+++ b/Base de Dados/Dados Tratados/NOVEMBRO_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\GitHub\Projeto-Painel-de-BI-Dados-Agricolas\Base de Dados\Dados Tratados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB4C557-812C-491F-A053-C8B8FB9FC58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94FF7EC-6B73-419A-9C4C-C5D778703D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1129,9 +1129,7 @@
     <tableColumn id="22" xr3:uid="{49B2C1E3-0396-4037-BB4B-32C18FDB6CC7}" name="CEVADA" dataDxfId="5"/>
     <tableColumn id="23" xr3:uid="{C10C34AB-D106-4FB2-B097-C90EF653E9E5}" name="TRIGO" dataDxfId="4"/>
     <tableColumn id="24" xr3:uid="{80045204-E6E2-42D6-9449-CCD3B9641988}" name="TRITICALE" dataDxfId="3"/>
-    <tableColumn id="25" xr3:uid="{0FB9C96B-75F4-4026-A109-A799A828C96B}" name="GERAL" dataDxfId="2">
-      <calculatedColumnFormula>SUM(B2,E2:F2,I2,M2:X2)</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="25" xr3:uid="{0FB9C96B-75F4-4026-A109-A799A828C96B}" name="GERAL" dataDxfId="2"/>
     <tableColumn id="26" xr3:uid="{FA0650E0-02EE-433A-927B-8DCFAD627C43}" name="ANO"/>
     <tableColumn id="27" xr3:uid="{94C00EC6-AB2D-4D90-B787-2C1FF57B5832}" name="MÊS" dataDxfId="1"/>
     <tableColumn id="28" xr3:uid="{57AFB38B-E07E-457A-9571-EB539326E109}" name="SAFRA" dataDxfId="0"/>
@@ -7629,7 +7627,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B2" sqref="B2:AJ25"/>
+      <selection pane="topRight" activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10677,8 +10675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BCD6B43-6B79-4F6C-BEBB-EEE94FDB59C5}">
   <dimension ref="A1:AM36"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:Y36"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13833,8 +13831,8 @@
   <dimension ref="A1:AM25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AD1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B2" sqref="B2:AJ25"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16712,143 +16710,108 @@
         <v>56</v>
       </c>
       <c r="B25" s="1">
-        <f>SUM(B2,B5:B6,B9,B13:B24)</f>
         <v>15267.900000000001</v>
       </c>
       <c r="C25" s="1">
-        <f t="shared" ref="C25:AJ25" si="0">SUM(C2,C5:C6,C9,C13:C24)</f>
         <v>544.29999999999995</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="0"/>
         <v>3305.4</v>
       </c>
       <c r="E25" s="1">
-        <f t="shared" si="0"/>
         <v>192.00000000000003</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" si="0"/>
         <v>36.599999999999994</v>
       </c>
       <c r="G25" s="1">
-        <f t="shared" si="0"/>
         <v>20.8</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" si="0"/>
         <v>4346.3999999999996</v>
       </c>
       <c r="I25" s="1">
-        <f t="shared" si="0"/>
         <v>6822.4000000000005</v>
       </c>
       <c r="J25" s="1">
-        <f t="shared" si="0"/>
         <v>28545.7</v>
       </c>
       <c r="K25" s="1">
-        <f t="shared" si="0"/>
         <v>7191.1</v>
       </c>
       <c r="L25" s="1">
-        <f t="shared" si="0"/>
         <v>6290.9</v>
       </c>
       <c r="M25" s="1">
-        <f t="shared" si="0"/>
         <v>676.59999999999991</v>
       </c>
       <c r="N25" s="1">
-        <f t="shared" si="0"/>
         <v>53.8</v>
       </c>
       <c r="O25" s="1">
-        <f t="shared" si="0"/>
         <v>113.2</v>
       </c>
       <c r="P25" s="1">
-        <f t="shared" si="0"/>
         <v>257.7</v>
       </c>
       <c r="Q25" s="1">
-        <f t="shared" si="0"/>
         <v>116.9</v>
       </c>
       <c r="R25" s="1">
-        <f t="shared" si="0"/>
         <v>998.7</v>
       </c>
       <c r="S25" s="1">
-        <f t="shared" si="0"/>
         <v>12846.8</v>
       </c>
       <c r="T25" s="1">
-        <f t="shared" si="0"/>
         <v>150383.19999999995</v>
       </c>
       <c r="U25" s="1">
-        <f t="shared" si="0"/>
         <v>92045.599999999991</v>
       </c>
       <c r="V25" s="1">
-        <f t="shared" si="0"/>
         <v>25195.799999999996</v>
       </c>
       <c r="W25" s="1">
-        <f t="shared" si="0"/>
         <v>32232.100000000002</v>
       </c>
       <c r="X25" s="1">
-        <f t="shared" si="0"/>
         <v>909.69999999999993</v>
       </c>
       <c r="Y25" s="1">
-        <f t="shared" si="0"/>
         <v>28481.500000000004</v>
       </c>
       <c r="Z25" s="1">
-        <f t="shared" si="0"/>
         <v>18374.800000000003</v>
       </c>
       <c r="AA25" s="1">
-        <f t="shared" si="0"/>
         <v>50.300000000000004</v>
       </c>
       <c r="AB25" s="1">
-        <f t="shared" si="0"/>
         <v>9.1</v>
       </c>
       <c r="AC25" s="1">
-        <f t="shared" si="0"/>
         <v>10047.299999999999</v>
       </c>
       <c r="AD25" s="1">
-        <f t="shared" si="0"/>
         <v>93337.099999999991</v>
       </c>
       <c r="AE25" s="1">
-        <f t="shared" si="0"/>
         <v>45277.599999999991</v>
       </c>
       <c r="AF25" s="1">
-        <f t="shared" si="0"/>
         <v>6979.2</v>
       </c>
       <c r="AG25" s="1">
-        <f t="shared" si="0"/>
         <v>41080.299999999981</v>
       </c>
       <c r="AH25" s="1">
-        <f t="shared" si="0"/>
         <v>43813.600000000006</v>
       </c>
       <c r="AI25" s="1">
-        <f t="shared" si="0"/>
         <v>272201.8</v>
       </c>
       <c r="AJ25" s="1">
-        <f t="shared" si="0"/>
         <v>316015.39999999997</v>
       </c>
       <c r="AK25" s="2">
@@ -16874,8 +16837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37856A1E-82E7-45AE-A2B0-C510B7D63887}">
   <dimension ref="A1:AM36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17070,7 +17033,6 @@
         <v>0</v>
       </c>
       <c r="Y2" s="1">
-        <f t="shared" ref="Y2:Y36" si="0">SUM(B2,E2:F2,I2,M2:X2)</f>
         <v>15267.900000000001</v>
       </c>
       <c r="Z2">
@@ -17157,7 +17119,6 @@
         <v>0</v>
       </c>
       <c r="Y3" s="1">
-        <f t="shared" si="0"/>
         <v>544.29999999999995</v>
       </c>
       <c r="Z3">
@@ -17244,7 +17205,6 @@
         <v>0</v>
       </c>
       <c r="Y4" s="1">
-        <f t="shared" si="0"/>
         <v>3305.4</v>
       </c>
       <c r="Z4">
@@ -17331,7 +17291,6 @@
         <v>0</v>
       </c>
       <c r="Y5" s="1">
-        <f t="shared" si="0"/>
         <v>192.00000000000003</v>
       </c>
       <c r="Z5">
@@ -17418,7 +17377,6 @@
         <v>0</v>
       </c>
       <c r="Y6" s="1">
-        <f t="shared" si="0"/>
         <v>36.599999999999994</v>
       </c>
       <c r="Z6">
@@ -17505,7 +17463,6 @@
         <v>0</v>
       </c>
       <c r="Y7" s="1">
-        <f t="shared" si="0"/>
         <v>20.8</v>
       </c>
       <c r="Z7">
@@ -17592,7 +17549,6 @@
         <v>0</v>
       </c>
       <c r="Y8" s="1">
-        <f t="shared" si="0"/>
         <v>4346.3999999999996</v>
       </c>
       <c r="Z8">
@@ -17679,7 +17635,6 @@
         <v>0</v>
       </c>
       <c r="Y9" s="1">
-        <f t="shared" si="0"/>
         <v>6822.4000000000005</v>
       </c>
       <c r="Z9">
@@ -17766,7 +17721,6 @@
         <v>0</v>
       </c>
       <c r="Y10" s="1">
-        <f t="shared" si="0"/>
         <v>28545.7</v>
       </c>
       <c r="Z10">
@@ -17853,7 +17807,6 @@
         <v>0</v>
       </c>
       <c r="Y11" s="1">
-        <f t="shared" si="0"/>
         <v>7191.1</v>
       </c>
       <c r="Z11">
@@ -17940,7 +17893,6 @@
         <v>0</v>
       </c>
       <c r="Y12" s="1">
-        <f t="shared" si="0"/>
         <v>6290.9</v>
       </c>
       <c r="Z12">
@@ -18027,7 +17979,6 @@
         <v>0</v>
       </c>
       <c r="Y13" s="1">
-        <f t="shared" si="0"/>
         <v>676.59999999999991</v>
       </c>
       <c r="Z13">
@@ -18114,7 +18065,6 @@
         <v>0</v>
       </c>
       <c r="Y14" s="1">
-        <f t="shared" si="0"/>
         <v>53.8</v>
       </c>
       <c r="Z14">
@@ -18201,7 +18151,6 @@
         <v>0</v>
       </c>
       <c r="Y15" s="1">
-        <f t="shared" si="0"/>
         <v>113.2</v>
       </c>
       <c r="Z15">
@@ -18288,7 +18237,6 @@
         <v>0</v>
       </c>
       <c r="Y16" s="1">
-        <f t="shared" si="0"/>
         <v>257.7</v>
       </c>
       <c r="Z16">
@@ -18375,7 +18323,6 @@
         <v>0</v>
       </c>
       <c r="Y17" s="1">
-        <f t="shared" si="0"/>
         <v>116.9</v>
       </c>
       <c r="Z17">
@@ -18462,7 +18409,6 @@
         <v>0</v>
       </c>
       <c r="Y18" s="1">
-        <f t="shared" si="0"/>
         <v>998.7</v>
       </c>
       <c r="Z18">
@@ -18549,7 +18495,6 @@
         <v>0</v>
       </c>
       <c r="Y19" s="1">
-        <f t="shared" si="0"/>
         <v>12846.8</v>
       </c>
       <c r="Z19">
@@ -18636,7 +18581,6 @@
         <v>0</v>
       </c>
       <c r="Y20" s="1">
-        <f t="shared" si="0"/>
         <v>150383.19999999995</v>
       </c>
       <c r="Z20">
@@ -18723,7 +18667,6 @@
         <v>0</v>
       </c>
       <c r="Y21" s="1">
-        <f t="shared" si="0"/>
         <v>92045.599999999991</v>
       </c>
       <c r="Z21">
@@ -18810,7 +18753,6 @@
         <v>0</v>
       </c>
       <c r="Y22" s="1">
-        <f t="shared" si="0"/>
         <v>25195.799999999996</v>
       </c>
       <c r="Z22">
@@ -18897,7 +18839,6 @@
         <v>0</v>
       </c>
       <c r="Y23" s="1">
-        <f t="shared" si="0"/>
         <v>32232.100000000002</v>
       </c>
       <c r="Z23">
@@ -18984,7 +18925,6 @@
         <v>0</v>
       </c>
       <c r="Y24" s="1">
-        <f t="shared" si="0"/>
         <v>909.69999999999993</v>
       </c>
       <c r="Z24">
@@ -19071,7 +19011,6 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="Y25" s="1">
-        <f t="shared" si="0"/>
         <v>28481.500000000004</v>
       </c>
       <c r="Z25">
@@ -19158,7 +19097,6 @@
         <v>0</v>
       </c>
       <c r="Y26" s="1">
-        <f t="shared" si="0"/>
         <v>18374.800000000003</v>
       </c>
       <c r="Z26">
@@ -19256,7 +19194,6 @@
         <v>0</v>
       </c>
       <c r="Y27" s="1">
-        <f t="shared" si="0"/>
         <v>50.300000000000004</v>
       </c>
       <c r="Z27">
@@ -19343,7 +19280,6 @@
         <v>0</v>
       </c>
       <c r="Y28" s="1">
-        <f t="shared" si="0"/>
         <v>9.1</v>
       </c>
       <c r="Z28">
@@ -19430,7 +19366,6 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="Y29" s="1">
-        <f t="shared" si="0"/>
         <v>10047.299999999999</v>
       </c>
       <c r="Z29">
@@ -19517,7 +19452,6 @@
         <v>52.900000000000006</v>
       </c>
       <c r="Y30" s="1">
-        <f t="shared" si="0"/>
         <v>93337.099999999991</v>
       </c>
       <c r="Z30">
@@ -19604,7 +19538,6 @@
         <v>34.200000000000003</v>
       </c>
       <c r="Y31" s="1">
-        <f t="shared" si="0"/>
         <v>45277.599999999991</v>
       </c>
       <c r="Z31">
@@ -19691,7 +19624,6 @@
         <v>0</v>
       </c>
       <c r="Y32" s="1">
-        <f t="shared" si="0"/>
         <v>6979.2</v>
       </c>
       <c r="Z32">
@@ -19778,7 +19710,6 @@
         <v>18.7</v>
       </c>
       <c r="Y33" s="1">
-        <f t="shared" si="0"/>
         <v>41080.299999999981</v>
       </c>
       <c r="Z33">
@@ -19865,7 +19796,6 @@
         <v>0</v>
       </c>
       <c r="Y34" s="1">
-        <f t="shared" si="0"/>
         <v>43813.600000000006</v>
       </c>
       <c r="Z34">
@@ -19952,7 +19882,6 @@
         <v>57.800000000000004</v>
       </c>
       <c r="Y35" s="1">
-        <f t="shared" si="0"/>
         <v>272201.8</v>
       </c>
       <c r="Z35">
@@ -20039,7 +19968,6 @@
         <v>57.800000000000004</v>
       </c>
       <c r="Y36" s="1">
-        <f t="shared" si="0"/>
         <v>316015.39999999997</v>
       </c>
       <c r="Z36">

</xml_diff>